<commit_message>
updates spreadsheets and ingest warnings
</commit_message>
<xml_diff>
--- a/xls/ObsidianInventory.xlsx
+++ b/xls/ObsidianInventory.xlsx
@@ -1,39 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cheitman2/Documents/BTSync/Grants/SPARC/SPARC Activities/Data Tables &amp; Schema/FINAL DB tables/March 2017 Final Tables/drive-download-20170328T141955Z-001/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Salmon\2018 DBs - Paul Fixes Late Feb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12020" yWindow="460" windowWidth="21580" windowHeight="13320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$WWH$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$75</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="490">
   <si>
     <t>SITE</t>
   </si>
@@ -1500,6 +1497,9 @@
   </si>
   <si>
     <t>General Site</t>
+  </si>
+  <si>
+    <t>C-2-5.3</t>
   </si>
 </sst>
 </file>
@@ -2069,1680 +2069,1680 @@
   <dimension ref="A1:AD82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="13" customWidth="1"/>
     <col min="5" max="5" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="35" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" style="35" customWidth="1"/>
     <col min="9" max="9" width="6" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="13" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" style="37" customWidth="1"/>
-    <col min="13" max="13" width="13.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="42" customWidth="1"/>
-    <col min="15" max="15" width="6.5" style="42" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" style="42" customWidth="1"/>
-    <col min="17" max="17" width="12.5" style="13" customWidth="1"/>
-    <col min="18" max="18" width="8.1640625" style="38" customWidth="1"/>
-    <col min="19" max="19" width="8.5" style="44" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="35" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" style="13" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="37" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="6.6328125" style="42" customWidth="1"/>
+    <col min="15" max="15" width="6.453125" style="42" customWidth="1"/>
+    <col min="16" max="16" width="6.36328125" style="42" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="8.1796875" style="38" customWidth="1"/>
+    <col min="19" max="19" width="8.453125" style="44" customWidth="1"/>
+    <col min="20" max="20" width="8.453125" style="35" customWidth="1"/>
+    <col min="21" max="21" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" style="38" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18" style="13" customWidth="1"/>
-    <col min="25" max="25" width="7.5" style="13" customWidth="1"/>
-    <col min="26" max="26" width="10.5" style="13" customWidth="1"/>
-    <col min="27" max="256" width="8.83203125" style="13"/>
-    <col min="257" max="257" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.453125" style="13" customWidth="1"/>
+    <col min="26" max="26" width="10.453125" style="13" customWidth="1"/>
+    <col min="27" max="256" width="8.81640625" style="13"/>
+    <col min="257" max="257" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="259" max="259" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="7.6640625" style="13" customWidth="1"/>
+    <col min="260" max="260" width="7.6328125" style="13" customWidth="1"/>
     <col min="261" max="261" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="262" max="262" width="8" style="13" customWidth="1"/>
     <col min="263" max="263" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="10.33203125" style="13" customWidth="1"/>
-    <col min="265" max="265" width="9.5" style="13" customWidth="1"/>
-    <col min="266" max="266" width="10.1640625" style="13" customWidth="1"/>
-    <col min="267" max="267" width="12.5" style="13" customWidth="1"/>
-    <col min="268" max="268" width="6.6640625" style="13" customWidth="1"/>
-    <col min="269" max="269" width="6.5" style="13" customWidth="1"/>
-    <col min="270" max="270" width="6.33203125" style="13" customWidth="1"/>
-    <col min="271" max="271" width="12.5" style="13" customWidth="1"/>
-    <col min="272" max="272" width="8.1640625" style="13" customWidth="1"/>
-    <col min="273" max="274" width="8.5" style="13" customWidth="1"/>
-    <col min="275" max="275" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="10.36328125" style="13" customWidth="1"/>
+    <col min="265" max="265" width="9.453125" style="13" customWidth="1"/>
+    <col min="266" max="266" width="10.1796875" style="13" customWidth="1"/>
+    <col min="267" max="267" width="12.453125" style="13" customWidth="1"/>
+    <col min="268" max="268" width="6.6328125" style="13" customWidth="1"/>
+    <col min="269" max="269" width="6.453125" style="13" customWidth="1"/>
+    <col min="270" max="270" width="6.36328125" style="13" customWidth="1"/>
+    <col min="271" max="271" width="12.453125" style="13" customWidth="1"/>
+    <col min="272" max="272" width="8.1796875" style="13" customWidth="1"/>
+    <col min="273" max="274" width="8.453125" style="13" customWidth="1"/>
+    <col min="275" max="275" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="278" max="278" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="280" max="280" width="18" style="13" customWidth="1"/>
-    <col min="281" max="281" width="7.5" style="13" customWidth="1"/>
-    <col min="282" max="282" width="10.5" style="13" customWidth="1"/>
-    <col min="283" max="512" width="8.83203125" style="13"/>
-    <col min="513" max="513" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="7.453125" style="13" customWidth="1"/>
+    <col min="282" max="282" width="10.453125" style="13" customWidth="1"/>
+    <col min="283" max="512" width="8.81640625" style="13"/>
+    <col min="513" max="513" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="515" max="515" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="516" max="516" width="7.6640625" style="13" customWidth="1"/>
+    <col min="516" max="516" width="7.6328125" style="13" customWidth="1"/>
     <col min="517" max="517" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="518" max="518" width="8" style="13" customWidth="1"/>
     <col min="519" max="519" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="10.33203125" style="13" customWidth="1"/>
-    <col min="521" max="521" width="9.5" style="13" customWidth="1"/>
-    <col min="522" max="522" width="10.1640625" style="13" customWidth="1"/>
-    <col min="523" max="523" width="12.5" style="13" customWidth="1"/>
-    <col min="524" max="524" width="6.6640625" style="13" customWidth="1"/>
-    <col min="525" max="525" width="6.5" style="13" customWidth="1"/>
-    <col min="526" max="526" width="6.33203125" style="13" customWidth="1"/>
-    <col min="527" max="527" width="12.5" style="13" customWidth="1"/>
-    <col min="528" max="528" width="8.1640625" style="13" customWidth="1"/>
-    <col min="529" max="530" width="8.5" style="13" customWidth="1"/>
-    <col min="531" max="531" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="532" max="532" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="533" max="533" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="10.36328125" style="13" customWidth="1"/>
+    <col min="521" max="521" width="9.453125" style="13" customWidth="1"/>
+    <col min="522" max="522" width="10.1796875" style="13" customWidth="1"/>
+    <col min="523" max="523" width="12.453125" style="13" customWidth="1"/>
+    <col min="524" max="524" width="6.6328125" style="13" customWidth="1"/>
+    <col min="525" max="525" width="6.453125" style="13" customWidth="1"/>
+    <col min="526" max="526" width="6.36328125" style="13" customWidth="1"/>
+    <col min="527" max="527" width="12.453125" style="13" customWidth="1"/>
+    <col min="528" max="528" width="8.1796875" style="13" customWidth="1"/>
+    <col min="529" max="530" width="8.453125" style="13" customWidth="1"/>
+    <col min="531" max="531" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="532" max="532" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="533" max="533" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="534" max="534" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="535" max="535" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="535" max="535" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="536" max="536" width="18" style="13" customWidth="1"/>
-    <col min="537" max="537" width="7.5" style="13" customWidth="1"/>
-    <col min="538" max="538" width="10.5" style="13" customWidth="1"/>
-    <col min="539" max="768" width="8.83203125" style="13"/>
-    <col min="769" max="769" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="537" max="537" width="7.453125" style="13" customWidth="1"/>
+    <col min="538" max="538" width="10.453125" style="13" customWidth="1"/>
+    <col min="539" max="768" width="8.81640625" style="13"/>
+    <col min="769" max="769" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="771" max="771" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="772" max="772" width="7.6640625" style="13" customWidth="1"/>
+    <col min="772" max="772" width="7.6328125" style="13" customWidth="1"/>
     <col min="773" max="773" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="774" max="774" width="8" style="13" customWidth="1"/>
     <col min="775" max="775" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="10.33203125" style="13" customWidth="1"/>
-    <col min="777" max="777" width="9.5" style="13" customWidth="1"/>
-    <col min="778" max="778" width="10.1640625" style="13" customWidth="1"/>
-    <col min="779" max="779" width="12.5" style="13" customWidth="1"/>
-    <col min="780" max="780" width="6.6640625" style="13" customWidth="1"/>
-    <col min="781" max="781" width="6.5" style="13" customWidth="1"/>
-    <col min="782" max="782" width="6.33203125" style="13" customWidth="1"/>
-    <col min="783" max="783" width="12.5" style="13" customWidth="1"/>
-    <col min="784" max="784" width="8.1640625" style="13" customWidth="1"/>
-    <col min="785" max="786" width="8.5" style="13" customWidth="1"/>
-    <col min="787" max="787" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="788" max="788" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="789" max="789" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="10.36328125" style="13" customWidth="1"/>
+    <col min="777" max="777" width="9.453125" style="13" customWidth="1"/>
+    <col min="778" max="778" width="10.1796875" style="13" customWidth="1"/>
+    <col min="779" max="779" width="12.453125" style="13" customWidth="1"/>
+    <col min="780" max="780" width="6.6328125" style="13" customWidth="1"/>
+    <col min="781" max="781" width="6.453125" style="13" customWidth="1"/>
+    <col min="782" max="782" width="6.36328125" style="13" customWidth="1"/>
+    <col min="783" max="783" width="12.453125" style="13" customWidth="1"/>
+    <col min="784" max="784" width="8.1796875" style="13" customWidth="1"/>
+    <col min="785" max="786" width="8.453125" style="13" customWidth="1"/>
+    <col min="787" max="787" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="788" max="788" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="789" max="789" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="790" max="790" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="791" max="791" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="791" max="791" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="792" max="792" width="18" style="13" customWidth="1"/>
-    <col min="793" max="793" width="7.5" style="13" customWidth="1"/>
-    <col min="794" max="794" width="10.5" style="13" customWidth="1"/>
-    <col min="795" max="1024" width="8.83203125" style="13"/>
-    <col min="1025" max="1025" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="793" max="793" width="7.453125" style="13" customWidth="1"/>
+    <col min="794" max="794" width="10.453125" style="13" customWidth="1"/>
+    <col min="795" max="1024" width="8.81640625" style="13"/>
+    <col min="1025" max="1025" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1027" max="1027" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1028" width="7.6640625" style="13" customWidth="1"/>
+    <col min="1028" max="1028" width="7.6328125" style="13" customWidth="1"/>
     <col min="1029" max="1029" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="1030" max="1030" width="8" style="13" customWidth="1"/>
     <col min="1031" max="1031" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="10.33203125" style="13" customWidth="1"/>
-    <col min="1033" max="1033" width="9.5" style="13" customWidth="1"/>
-    <col min="1034" max="1034" width="10.1640625" style="13" customWidth="1"/>
-    <col min="1035" max="1035" width="12.5" style="13" customWidth="1"/>
-    <col min="1036" max="1036" width="6.6640625" style="13" customWidth="1"/>
-    <col min="1037" max="1037" width="6.5" style="13" customWidth="1"/>
-    <col min="1038" max="1038" width="6.33203125" style="13" customWidth="1"/>
-    <col min="1039" max="1039" width="12.5" style="13" customWidth="1"/>
-    <col min="1040" max="1040" width="8.1640625" style="13" customWidth="1"/>
-    <col min="1041" max="1042" width="8.5" style="13" customWidth="1"/>
-    <col min="1043" max="1043" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1044" max="1044" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1045" max="1045" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="10.36328125" style="13" customWidth="1"/>
+    <col min="1033" max="1033" width="9.453125" style="13" customWidth="1"/>
+    <col min="1034" max="1034" width="10.1796875" style="13" customWidth="1"/>
+    <col min="1035" max="1035" width="12.453125" style="13" customWidth="1"/>
+    <col min="1036" max="1036" width="6.6328125" style="13" customWidth="1"/>
+    <col min="1037" max="1037" width="6.453125" style="13" customWidth="1"/>
+    <col min="1038" max="1038" width="6.36328125" style="13" customWidth="1"/>
+    <col min="1039" max="1039" width="12.453125" style="13" customWidth="1"/>
+    <col min="1040" max="1040" width="8.1796875" style="13" customWidth="1"/>
+    <col min="1041" max="1042" width="8.453125" style="13" customWidth="1"/>
+    <col min="1043" max="1043" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1044" max="1044" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1045" max="1045" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="1046" max="1046" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="1047" max="1047" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1047" max="1047" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1048" max="1048" width="18" style="13" customWidth="1"/>
-    <col min="1049" max="1049" width="7.5" style="13" customWidth="1"/>
-    <col min="1050" max="1050" width="10.5" style="13" customWidth="1"/>
-    <col min="1051" max="1280" width="8.83203125" style="13"/>
-    <col min="1281" max="1281" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1049" width="7.453125" style="13" customWidth="1"/>
+    <col min="1050" max="1050" width="10.453125" style="13" customWidth="1"/>
+    <col min="1051" max="1280" width="8.81640625" style="13"/>
+    <col min="1281" max="1281" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1283" max="1283" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="1284" max="1284" width="7.6640625" style="13" customWidth="1"/>
+    <col min="1284" max="1284" width="7.6328125" style="13" customWidth="1"/>
     <col min="1285" max="1285" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="1286" max="1286" width="8" style="13" customWidth="1"/>
     <col min="1287" max="1287" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="10.33203125" style="13" customWidth="1"/>
-    <col min="1289" max="1289" width="9.5" style="13" customWidth="1"/>
-    <col min="1290" max="1290" width="10.1640625" style="13" customWidth="1"/>
-    <col min="1291" max="1291" width="12.5" style="13" customWidth="1"/>
-    <col min="1292" max="1292" width="6.6640625" style="13" customWidth="1"/>
-    <col min="1293" max="1293" width="6.5" style="13" customWidth="1"/>
-    <col min="1294" max="1294" width="6.33203125" style="13" customWidth="1"/>
-    <col min="1295" max="1295" width="12.5" style="13" customWidth="1"/>
-    <col min="1296" max="1296" width="8.1640625" style="13" customWidth="1"/>
-    <col min="1297" max="1298" width="8.5" style="13" customWidth="1"/>
-    <col min="1299" max="1299" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1300" max="1300" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1301" max="1301" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="10.36328125" style="13" customWidth="1"/>
+    <col min="1289" max="1289" width="9.453125" style="13" customWidth="1"/>
+    <col min="1290" max="1290" width="10.1796875" style="13" customWidth="1"/>
+    <col min="1291" max="1291" width="12.453125" style="13" customWidth="1"/>
+    <col min="1292" max="1292" width="6.6328125" style="13" customWidth="1"/>
+    <col min="1293" max="1293" width="6.453125" style="13" customWidth="1"/>
+    <col min="1294" max="1294" width="6.36328125" style="13" customWidth="1"/>
+    <col min="1295" max="1295" width="12.453125" style="13" customWidth="1"/>
+    <col min="1296" max="1296" width="8.1796875" style="13" customWidth="1"/>
+    <col min="1297" max="1298" width="8.453125" style="13" customWidth="1"/>
+    <col min="1299" max="1299" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1300" max="1300" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1301" max="1301" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="1302" max="1302" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="1303" max="1303" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1303" max="1303" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1304" max="1304" width="18" style="13" customWidth="1"/>
-    <col min="1305" max="1305" width="7.5" style="13" customWidth="1"/>
-    <col min="1306" max="1306" width="10.5" style="13" customWidth="1"/>
-    <col min="1307" max="1536" width="8.83203125" style="13"/>
-    <col min="1537" max="1537" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1305" width="7.453125" style="13" customWidth="1"/>
+    <col min="1306" max="1306" width="10.453125" style="13" customWidth="1"/>
+    <col min="1307" max="1536" width="8.81640625" style="13"/>
+    <col min="1537" max="1537" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1539" max="1539" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="1540" max="1540" width="7.6640625" style="13" customWidth="1"/>
+    <col min="1540" max="1540" width="7.6328125" style="13" customWidth="1"/>
     <col min="1541" max="1541" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="1542" max="1542" width="8" style="13" customWidth="1"/>
     <col min="1543" max="1543" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="10.33203125" style="13" customWidth="1"/>
-    <col min="1545" max="1545" width="9.5" style="13" customWidth="1"/>
-    <col min="1546" max="1546" width="10.1640625" style="13" customWidth="1"/>
-    <col min="1547" max="1547" width="12.5" style="13" customWidth="1"/>
-    <col min="1548" max="1548" width="6.6640625" style="13" customWidth="1"/>
-    <col min="1549" max="1549" width="6.5" style="13" customWidth="1"/>
-    <col min="1550" max="1550" width="6.33203125" style="13" customWidth="1"/>
-    <col min="1551" max="1551" width="12.5" style="13" customWidth="1"/>
-    <col min="1552" max="1552" width="8.1640625" style="13" customWidth="1"/>
-    <col min="1553" max="1554" width="8.5" style="13" customWidth="1"/>
-    <col min="1555" max="1555" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1556" max="1556" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1557" max="1557" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="10.36328125" style="13" customWidth="1"/>
+    <col min="1545" max="1545" width="9.453125" style="13" customWidth="1"/>
+    <col min="1546" max="1546" width="10.1796875" style="13" customWidth="1"/>
+    <col min="1547" max="1547" width="12.453125" style="13" customWidth="1"/>
+    <col min="1548" max="1548" width="6.6328125" style="13" customWidth="1"/>
+    <col min="1549" max="1549" width="6.453125" style="13" customWidth="1"/>
+    <col min="1550" max="1550" width="6.36328125" style="13" customWidth="1"/>
+    <col min="1551" max="1551" width="12.453125" style="13" customWidth="1"/>
+    <col min="1552" max="1552" width="8.1796875" style="13" customWidth="1"/>
+    <col min="1553" max="1554" width="8.453125" style="13" customWidth="1"/>
+    <col min="1555" max="1555" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1556" max="1556" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1557" max="1557" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="1558" max="1558" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="1559" max="1559" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1559" max="1559" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1560" max="1560" width="18" style="13" customWidth="1"/>
-    <col min="1561" max="1561" width="7.5" style="13" customWidth="1"/>
-    <col min="1562" max="1562" width="10.5" style="13" customWidth="1"/>
-    <col min="1563" max="1792" width="8.83203125" style="13"/>
-    <col min="1793" max="1793" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1561" width="7.453125" style="13" customWidth="1"/>
+    <col min="1562" max="1562" width="10.453125" style="13" customWidth="1"/>
+    <col min="1563" max="1792" width="8.81640625" style="13"/>
+    <col min="1793" max="1793" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1795" max="1795" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="1796" max="1796" width="7.6640625" style="13" customWidth="1"/>
+    <col min="1796" max="1796" width="7.6328125" style="13" customWidth="1"/>
     <col min="1797" max="1797" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="1798" max="1798" width="8" style="13" customWidth="1"/>
     <col min="1799" max="1799" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="10.33203125" style="13" customWidth="1"/>
-    <col min="1801" max="1801" width="9.5" style="13" customWidth="1"/>
-    <col min="1802" max="1802" width="10.1640625" style="13" customWidth="1"/>
-    <col min="1803" max="1803" width="12.5" style="13" customWidth="1"/>
-    <col min="1804" max="1804" width="6.6640625" style="13" customWidth="1"/>
-    <col min="1805" max="1805" width="6.5" style="13" customWidth="1"/>
-    <col min="1806" max="1806" width="6.33203125" style="13" customWidth="1"/>
-    <col min="1807" max="1807" width="12.5" style="13" customWidth="1"/>
-    <col min="1808" max="1808" width="8.1640625" style="13" customWidth="1"/>
-    <col min="1809" max="1810" width="8.5" style="13" customWidth="1"/>
-    <col min="1811" max="1811" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="1812" max="1812" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="1813" max="1813" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="10.36328125" style="13" customWidth="1"/>
+    <col min="1801" max="1801" width="9.453125" style="13" customWidth="1"/>
+    <col min="1802" max="1802" width="10.1796875" style="13" customWidth="1"/>
+    <col min="1803" max="1803" width="12.453125" style="13" customWidth="1"/>
+    <col min="1804" max="1804" width="6.6328125" style="13" customWidth="1"/>
+    <col min="1805" max="1805" width="6.453125" style="13" customWidth="1"/>
+    <col min="1806" max="1806" width="6.36328125" style="13" customWidth="1"/>
+    <col min="1807" max="1807" width="12.453125" style="13" customWidth="1"/>
+    <col min="1808" max="1808" width="8.1796875" style="13" customWidth="1"/>
+    <col min="1809" max="1810" width="8.453125" style="13" customWidth="1"/>
+    <col min="1811" max="1811" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1812" max="1812" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1813" max="1813" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="1814" max="1814" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="1815" max="1815" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1815" max="1815" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="1816" max="1816" width="18" style="13" customWidth="1"/>
-    <col min="1817" max="1817" width="7.5" style="13" customWidth="1"/>
-    <col min="1818" max="1818" width="10.5" style="13" customWidth="1"/>
-    <col min="1819" max="2048" width="8.83203125" style="13"/>
-    <col min="2049" max="2049" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="1817" max="1817" width="7.453125" style="13" customWidth="1"/>
+    <col min="1818" max="1818" width="10.453125" style="13" customWidth="1"/>
+    <col min="1819" max="2048" width="8.81640625" style="13"/>
+    <col min="2049" max="2049" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2051" max="2051" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="2052" max="2052" width="7.6640625" style="13" customWidth="1"/>
+    <col min="2052" max="2052" width="7.6328125" style="13" customWidth="1"/>
     <col min="2053" max="2053" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="2054" max="2054" width="8" style="13" customWidth="1"/>
     <col min="2055" max="2055" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="10.33203125" style="13" customWidth="1"/>
-    <col min="2057" max="2057" width="9.5" style="13" customWidth="1"/>
-    <col min="2058" max="2058" width="10.1640625" style="13" customWidth="1"/>
-    <col min="2059" max="2059" width="12.5" style="13" customWidth="1"/>
-    <col min="2060" max="2060" width="6.6640625" style="13" customWidth="1"/>
-    <col min="2061" max="2061" width="6.5" style="13" customWidth="1"/>
-    <col min="2062" max="2062" width="6.33203125" style="13" customWidth="1"/>
-    <col min="2063" max="2063" width="12.5" style="13" customWidth="1"/>
-    <col min="2064" max="2064" width="8.1640625" style="13" customWidth="1"/>
-    <col min="2065" max="2066" width="8.5" style="13" customWidth="1"/>
-    <col min="2067" max="2067" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2068" max="2068" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2069" max="2069" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="10.36328125" style="13" customWidth="1"/>
+    <col min="2057" max="2057" width="9.453125" style="13" customWidth="1"/>
+    <col min="2058" max="2058" width="10.1796875" style="13" customWidth="1"/>
+    <col min="2059" max="2059" width="12.453125" style="13" customWidth="1"/>
+    <col min="2060" max="2060" width="6.6328125" style="13" customWidth="1"/>
+    <col min="2061" max="2061" width="6.453125" style="13" customWidth="1"/>
+    <col min="2062" max="2062" width="6.36328125" style="13" customWidth="1"/>
+    <col min="2063" max="2063" width="12.453125" style="13" customWidth="1"/>
+    <col min="2064" max="2064" width="8.1796875" style="13" customWidth="1"/>
+    <col min="2065" max="2066" width="8.453125" style="13" customWidth="1"/>
+    <col min="2067" max="2067" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2068" max="2068" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2069" max="2069" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="2070" max="2070" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="2071" max="2071" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2071" max="2071" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2072" max="2072" width="18" style="13" customWidth="1"/>
-    <col min="2073" max="2073" width="7.5" style="13" customWidth="1"/>
-    <col min="2074" max="2074" width="10.5" style="13" customWidth="1"/>
-    <col min="2075" max="2304" width="8.83203125" style="13"/>
-    <col min="2305" max="2305" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2073" width="7.453125" style="13" customWidth="1"/>
+    <col min="2074" max="2074" width="10.453125" style="13" customWidth="1"/>
+    <col min="2075" max="2304" width="8.81640625" style="13"/>
+    <col min="2305" max="2305" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2307" max="2307" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="2308" max="2308" width="7.6640625" style="13" customWidth="1"/>
+    <col min="2308" max="2308" width="7.6328125" style="13" customWidth="1"/>
     <col min="2309" max="2309" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="2310" max="2310" width="8" style="13" customWidth="1"/>
     <col min="2311" max="2311" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="10.33203125" style="13" customWidth="1"/>
-    <col min="2313" max="2313" width="9.5" style="13" customWidth="1"/>
-    <col min="2314" max="2314" width="10.1640625" style="13" customWidth="1"/>
-    <col min="2315" max="2315" width="12.5" style="13" customWidth="1"/>
-    <col min="2316" max="2316" width="6.6640625" style="13" customWidth="1"/>
-    <col min="2317" max="2317" width="6.5" style="13" customWidth="1"/>
-    <col min="2318" max="2318" width="6.33203125" style="13" customWidth="1"/>
-    <col min="2319" max="2319" width="12.5" style="13" customWidth="1"/>
-    <col min="2320" max="2320" width="8.1640625" style="13" customWidth="1"/>
-    <col min="2321" max="2322" width="8.5" style="13" customWidth="1"/>
-    <col min="2323" max="2323" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2324" max="2324" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2325" max="2325" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="10.36328125" style="13" customWidth="1"/>
+    <col min="2313" max="2313" width="9.453125" style="13" customWidth="1"/>
+    <col min="2314" max="2314" width="10.1796875" style="13" customWidth="1"/>
+    <col min="2315" max="2315" width="12.453125" style="13" customWidth="1"/>
+    <col min="2316" max="2316" width="6.6328125" style="13" customWidth="1"/>
+    <col min="2317" max="2317" width="6.453125" style="13" customWidth="1"/>
+    <col min="2318" max="2318" width="6.36328125" style="13" customWidth="1"/>
+    <col min="2319" max="2319" width="12.453125" style="13" customWidth="1"/>
+    <col min="2320" max="2320" width="8.1796875" style="13" customWidth="1"/>
+    <col min="2321" max="2322" width="8.453125" style="13" customWidth="1"/>
+    <col min="2323" max="2323" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2324" max="2324" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2325" max="2325" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="2326" max="2326" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="2327" max="2327" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2327" max="2327" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2328" max="2328" width="18" style="13" customWidth="1"/>
-    <col min="2329" max="2329" width="7.5" style="13" customWidth="1"/>
-    <col min="2330" max="2330" width="10.5" style="13" customWidth="1"/>
-    <col min="2331" max="2560" width="8.83203125" style="13"/>
-    <col min="2561" max="2561" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2329" width="7.453125" style="13" customWidth="1"/>
+    <col min="2330" max="2330" width="10.453125" style="13" customWidth="1"/>
+    <col min="2331" max="2560" width="8.81640625" style="13"/>
+    <col min="2561" max="2561" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2563" max="2563" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="2564" max="2564" width="7.6640625" style="13" customWidth="1"/>
+    <col min="2564" max="2564" width="7.6328125" style="13" customWidth="1"/>
     <col min="2565" max="2565" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="2566" max="2566" width="8" style="13" customWidth="1"/>
     <col min="2567" max="2567" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="10.33203125" style="13" customWidth="1"/>
-    <col min="2569" max="2569" width="9.5" style="13" customWidth="1"/>
-    <col min="2570" max="2570" width="10.1640625" style="13" customWidth="1"/>
-    <col min="2571" max="2571" width="12.5" style="13" customWidth="1"/>
-    <col min="2572" max="2572" width="6.6640625" style="13" customWidth="1"/>
-    <col min="2573" max="2573" width="6.5" style="13" customWidth="1"/>
-    <col min="2574" max="2574" width="6.33203125" style="13" customWidth="1"/>
-    <col min="2575" max="2575" width="12.5" style="13" customWidth="1"/>
-    <col min="2576" max="2576" width="8.1640625" style="13" customWidth="1"/>
-    <col min="2577" max="2578" width="8.5" style="13" customWidth="1"/>
-    <col min="2579" max="2579" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2580" max="2580" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2581" max="2581" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="10.36328125" style="13" customWidth="1"/>
+    <col min="2569" max="2569" width="9.453125" style="13" customWidth="1"/>
+    <col min="2570" max="2570" width="10.1796875" style="13" customWidth="1"/>
+    <col min="2571" max="2571" width="12.453125" style="13" customWidth="1"/>
+    <col min="2572" max="2572" width="6.6328125" style="13" customWidth="1"/>
+    <col min="2573" max="2573" width="6.453125" style="13" customWidth="1"/>
+    <col min="2574" max="2574" width="6.36328125" style="13" customWidth="1"/>
+    <col min="2575" max="2575" width="12.453125" style="13" customWidth="1"/>
+    <col min="2576" max="2576" width="8.1796875" style="13" customWidth="1"/>
+    <col min="2577" max="2578" width="8.453125" style="13" customWidth="1"/>
+    <col min="2579" max="2579" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2580" max="2580" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2581" max="2581" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="2582" max="2582" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="2583" max="2583" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2583" max="2583" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2584" max="2584" width="18" style="13" customWidth="1"/>
-    <col min="2585" max="2585" width="7.5" style="13" customWidth="1"/>
-    <col min="2586" max="2586" width="10.5" style="13" customWidth="1"/>
-    <col min="2587" max="2816" width="8.83203125" style="13"/>
-    <col min="2817" max="2817" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2585" width="7.453125" style="13" customWidth="1"/>
+    <col min="2586" max="2586" width="10.453125" style="13" customWidth="1"/>
+    <col min="2587" max="2816" width="8.81640625" style="13"/>
+    <col min="2817" max="2817" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2819" max="2819" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="2820" max="2820" width="7.6640625" style="13" customWidth="1"/>
+    <col min="2820" max="2820" width="7.6328125" style="13" customWidth="1"/>
     <col min="2821" max="2821" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="2822" max="2822" width="8" style="13" customWidth="1"/>
     <col min="2823" max="2823" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="10.33203125" style="13" customWidth="1"/>
-    <col min="2825" max="2825" width="9.5" style="13" customWidth="1"/>
-    <col min="2826" max="2826" width="10.1640625" style="13" customWidth="1"/>
-    <col min="2827" max="2827" width="12.5" style="13" customWidth="1"/>
-    <col min="2828" max="2828" width="6.6640625" style="13" customWidth="1"/>
-    <col min="2829" max="2829" width="6.5" style="13" customWidth="1"/>
-    <col min="2830" max="2830" width="6.33203125" style="13" customWidth="1"/>
-    <col min="2831" max="2831" width="12.5" style="13" customWidth="1"/>
-    <col min="2832" max="2832" width="8.1640625" style="13" customWidth="1"/>
-    <col min="2833" max="2834" width="8.5" style="13" customWidth="1"/>
-    <col min="2835" max="2835" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2836" max="2836" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2837" max="2837" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="10.36328125" style="13" customWidth="1"/>
+    <col min="2825" max="2825" width="9.453125" style="13" customWidth="1"/>
+    <col min="2826" max="2826" width="10.1796875" style="13" customWidth="1"/>
+    <col min="2827" max="2827" width="12.453125" style="13" customWidth="1"/>
+    <col min="2828" max="2828" width="6.6328125" style="13" customWidth="1"/>
+    <col min="2829" max="2829" width="6.453125" style="13" customWidth="1"/>
+    <col min="2830" max="2830" width="6.36328125" style="13" customWidth="1"/>
+    <col min="2831" max="2831" width="12.453125" style="13" customWidth="1"/>
+    <col min="2832" max="2832" width="8.1796875" style="13" customWidth="1"/>
+    <col min="2833" max="2834" width="8.453125" style="13" customWidth="1"/>
+    <col min="2835" max="2835" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2836" max="2836" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2837" max="2837" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="2838" max="2838" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="2839" max="2839" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2839" max="2839" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="2840" max="2840" width="18" style="13" customWidth="1"/>
-    <col min="2841" max="2841" width="7.5" style="13" customWidth="1"/>
-    <col min="2842" max="2842" width="10.5" style="13" customWidth="1"/>
-    <col min="2843" max="3072" width="8.83203125" style="13"/>
-    <col min="3073" max="3073" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2841" max="2841" width="7.453125" style="13" customWidth="1"/>
+    <col min="2842" max="2842" width="10.453125" style="13" customWidth="1"/>
+    <col min="2843" max="3072" width="8.81640625" style="13"/>
+    <col min="3073" max="3073" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3075" max="3075" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="3076" max="3076" width="7.6640625" style="13" customWidth="1"/>
+    <col min="3076" max="3076" width="7.6328125" style="13" customWidth="1"/>
     <col min="3077" max="3077" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="3078" max="3078" width="8" style="13" customWidth="1"/>
     <col min="3079" max="3079" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="10.33203125" style="13" customWidth="1"/>
-    <col min="3081" max="3081" width="9.5" style="13" customWidth="1"/>
-    <col min="3082" max="3082" width="10.1640625" style="13" customWidth="1"/>
-    <col min="3083" max="3083" width="12.5" style="13" customWidth="1"/>
-    <col min="3084" max="3084" width="6.6640625" style="13" customWidth="1"/>
-    <col min="3085" max="3085" width="6.5" style="13" customWidth="1"/>
-    <col min="3086" max="3086" width="6.33203125" style="13" customWidth="1"/>
-    <col min="3087" max="3087" width="12.5" style="13" customWidth="1"/>
-    <col min="3088" max="3088" width="8.1640625" style="13" customWidth="1"/>
-    <col min="3089" max="3090" width="8.5" style="13" customWidth="1"/>
-    <col min="3091" max="3091" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3092" max="3092" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3093" max="3093" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="10.36328125" style="13" customWidth="1"/>
+    <col min="3081" max="3081" width="9.453125" style="13" customWidth="1"/>
+    <col min="3082" max="3082" width="10.1796875" style="13" customWidth="1"/>
+    <col min="3083" max="3083" width="12.453125" style="13" customWidth="1"/>
+    <col min="3084" max="3084" width="6.6328125" style="13" customWidth="1"/>
+    <col min="3085" max="3085" width="6.453125" style="13" customWidth="1"/>
+    <col min="3086" max="3086" width="6.36328125" style="13" customWidth="1"/>
+    <col min="3087" max="3087" width="12.453125" style="13" customWidth="1"/>
+    <col min="3088" max="3088" width="8.1796875" style="13" customWidth="1"/>
+    <col min="3089" max="3090" width="8.453125" style="13" customWidth="1"/>
+    <col min="3091" max="3091" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3092" max="3092" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3093" max="3093" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="3094" max="3094" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="3095" max="3095" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3095" max="3095" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3096" max="3096" width="18" style="13" customWidth="1"/>
-    <col min="3097" max="3097" width="7.5" style="13" customWidth="1"/>
-    <col min="3098" max="3098" width="10.5" style="13" customWidth="1"/>
-    <col min="3099" max="3328" width="8.83203125" style="13"/>
-    <col min="3329" max="3329" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3097" width="7.453125" style="13" customWidth="1"/>
+    <col min="3098" max="3098" width="10.453125" style="13" customWidth="1"/>
+    <col min="3099" max="3328" width="8.81640625" style="13"/>
+    <col min="3329" max="3329" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3331" max="3331" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="3332" max="3332" width="7.6640625" style="13" customWidth="1"/>
+    <col min="3332" max="3332" width="7.6328125" style="13" customWidth="1"/>
     <col min="3333" max="3333" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="3334" max="3334" width="8" style="13" customWidth="1"/>
     <col min="3335" max="3335" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="10.33203125" style="13" customWidth="1"/>
-    <col min="3337" max="3337" width="9.5" style="13" customWidth="1"/>
-    <col min="3338" max="3338" width="10.1640625" style="13" customWidth="1"/>
-    <col min="3339" max="3339" width="12.5" style="13" customWidth="1"/>
-    <col min="3340" max="3340" width="6.6640625" style="13" customWidth="1"/>
-    <col min="3341" max="3341" width="6.5" style="13" customWidth="1"/>
-    <col min="3342" max="3342" width="6.33203125" style="13" customWidth="1"/>
-    <col min="3343" max="3343" width="12.5" style="13" customWidth="1"/>
-    <col min="3344" max="3344" width="8.1640625" style="13" customWidth="1"/>
-    <col min="3345" max="3346" width="8.5" style="13" customWidth="1"/>
-    <col min="3347" max="3347" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3348" max="3348" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3349" max="3349" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="10.36328125" style="13" customWidth="1"/>
+    <col min="3337" max="3337" width="9.453125" style="13" customWidth="1"/>
+    <col min="3338" max="3338" width="10.1796875" style="13" customWidth="1"/>
+    <col min="3339" max="3339" width="12.453125" style="13" customWidth="1"/>
+    <col min="3340" max="3340" width="6.6328125" style="13" customWidth="1"/>
+    <col min="3341" max="3341" width="6.453125" style="13" customWidth="1"/>
+    <col min="3342" max="3342" width="6.36328125" style="13" customWidth="1"/>
+    <col min="3343" max="3343" width="12.453125" style="13" customWidth="1"/>
+    <col min="3344" max="3344" width="8.1796875" style="13" customWidth="1"/>
+    <col min="3345" max="3346" width="8.453125" style="13" customWidth="1"/>
+    <col min="3347" max="3347" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3348" max="3348" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3349" max="3349" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="3350" max="3350" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="3351" max="3351" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3351" max="3351" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3352" max="3352" width="18" style="13" customWidth="1"/>
-    <col min="3353" max="3353" width="7.5" style="13" customWidth="1"/>
-    <col min="3354" max="3354" width="10.5" style="13" customWidth="1"/>
-    <col min="3355" max="3584" width="8.83203125" style="13"/>
-    <col min="3585" max="3585" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3353" width="7.453125" style="13" customWidth="1"/>
+    <col min="3354" max="3354" width="10.453125" style="13" customWidth="1"/>
+    <col min="3355" max="3584" width="8.81640625" style="13"/>
+    <col min="3585" max="3585" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3587" max="3587" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="3588" max="3588" width="7.6640625" style="13" customWidth="1"/>
+    <col min="3588" max="3588" width="7.6328125" style="13" customWidth="1"/>
     <col min="3589" max="3589" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="3590" max="3590" width="8" style="13" customWidth="1"/>
     <col min="3591" max="3591" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="10.33203125" style="13" customWidth="1"/>
-    <col min="3593" max="3593" width="9.5" style="13" customWidth="1"/>
-    <col min="3594" max="3594" width="10.1640625" style="13" customWidth="1"/>
-    <col min="3595" max="3595" width="12.5" style="13" customWidth="1"/>
-    <col min="3596" max="3596" width="6.6640625" style="13" customWidth="1"/>
-    <col min="3597" max="3597" width="6.5" style="13" customWidth="1"/>
-    <col min="3598" max="3598" width="6.33203125" style="13" customWidth="1"/>
-    <col min="3599" max="3599" width="12.5" style="13" customWidth="1"/>
-    <col min="3600" max="3600" width="8.1640625" style="13" customWidth="1"/>
-    <col min="3601" max="3602" width="8.5" style="13" customWidth="1"/>
-    <col min="3603" max="3603" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3604" max="3604" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3605" max="3605" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="10.36328125" style="13" customWidth="1"/>
+    <col min="3593" max="3593" width="9.453125" style="13" customWidth="1"/>
+    <col min="3594" max="3594" width="10.1796875" style="13" customWidth="1"/>
+    <col min="3595" max="3595" width="12.453125" style="13" customWidth="1"/>
+    <col min="3596" max="3596" width="6.6328125" style="13" customWidth="1"/>
+    <col min="3597" max="3597" width="6.453125" style="13" customWidth="1"/>
+    <col min="3598" max="3598" width="6.36328125" style="13" customWidth="1"/>
+    <col min="3599" max="3599" width="12.453125" style="13" customWidth="1"/>
+    <col min="3600" max="3600" width="8.1796875" style="13" customWidth="1"/>
+    <col min="3601" max="3602" width="8.453125" style="13" customWidth="1"/>
+    <col min="3603" max="3603" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3604" max="3604" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3605" max="3605" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="3606" max="3606" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="3607" max="3607" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3607" max="3607" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3608" max="3608" width="18" style="13" customWidth="1"/>
-    <col min="3609" max="3609" width="7.5" style="13" customWidth="1"/>
-    <col min="3610" max="3610" width="10.5" style="13" customWidth="1"/>
-    <col min="3611" max="3840" width="8.83203125" style="13"/>
-    <col min="3841" max="3841" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3609" width="7.453125" style="13" customWidth="1"/>
+    <col min="3610" max="3610" width="10.453125" style="13" customWidth="1"/>
+    <col min="3611" max="3840" width="8.81640625" style="13"/>
+    <col min="3841" max="3841" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3843" max="3843" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="3844" max="3844" width="7.6640625" style="13" customWidth="1"/>
+    <col min="3844" max="3844" width="7.6328125" style="13" customWidth="1"/>
     <col min="3845" max="3845" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="3846" max="3846" width="8" style="13" customWidth="1"/>
     <col min="3847" max="3847" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="10.33203125" style="13" customWidth="1"/>
-    <col min="3849" max="3849" width="9.5" style="13" customWidth="1"/>
-    <col min="3850" max="3850" width="10.1640625" style="13" customWidth="1"/>
-    <col min="3851" max="3851" width="12.5" style="13" customWidth="1"/>
-    <col min="3852" max="3852" width="6.6640625" style="13" customWidth="1"/>
-    <col min="3853" max="3853" width="6.5" style="13" customWidth="1"/>
-    <col min="3854" max="3854" width="6.33203125" style="13" customWidth="1"/>
-    <col min="3855" max="3855" width="12.5" style="13" customWidth="1"/>
-    <col min="3856" max="3856" width="8.1640625" style="13" customWidth="1"/>
-    <col min="3857" max="3858" width="8.5" style="13" customWidth="1"/>
-    <col min="3859" max="3859" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3860" max="3860" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3861" max="3861" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="10.36328125" style="13" customWidth="1"/>
+    <col min="3849" max="3849" width="9.453125" style="13" customWidth="1"/>
+    <col min="3850" max="3850" width="10.1796875" style="13" customWidth="1"/>
+    <col min="3851" max="3851" width="12.453125" style="13" customWidth="1"/>
+    <col min="3852" max="3852" width="6.6328125" style="13" customWidth="1"/>
+    <col min="3853" max="3853" width="6.453125" style="13" customWidth="1"/>
+    <col min="3854" max="3854" width="6.36328125" style="13" customWidth="1"/>
+    <col min="3855" max="3855" width="12.453125" style="13" customWidth="1"/>
+    <col min="3856" max="3856" width="8.1796875" style="13" customWidth="1"/>
+    <col min="3857" max="3858" width="8.453125" style="13" customWidth="1"/>
+    <col min="3859" max="3859" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3860" max="3860" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3861" max="3861" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="3862" max="3862" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="3863" max="3863" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3863" max="3863" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="3864" max="3864" width="18" style="13" customWidth="1"/>
-    <col min="3865" max="3865" width="7.5" style="13" customWidth="1"/>
-    <col min="3866" max="3866" width="10.5" style="13" customWidth="1"/>
-    <col min="3867" max="4096" width="8.83203125" style="13"/>
-    <col min="4097" max="4097" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3865" max="3865" width="7.453125" style="13" customWidth="1"/>
+    <col min="3866" max="3866" width="10.453125" style="13" customWidth="1"/>
+    <col min="3867" max="4096" width="8.81640625" style="13"/>
+    <col min="4097" max="4097" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4099" max="4099" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="4100" max="4100" width="7.6640625" style="13" customWidth="1"/>
+    <col min="4100" max="4100" width="7.6328125" style="13" customWidth="1"/>
     <col min="4101" max="4101" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="4102" max="4102" width="8" style="13" customWidth="1"/>
     <col min="4103" max="4103" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="10.33203125" style="13" customWidth="1"/>
-    <col min="4105" max="4105" width="9.5" style="13" customWidth="1"/>
-    <col min="4106" max="4106" width="10.1640625" style="13" customWidth="1"/>
-    <col min="4107" max="4107" width="12.5" style="13" customWidth="1"/>
-    <col min="4108" max="4108" width="6.6640625" style="13" customWidth="1"/>
-    <col min="4109" max="4109" width="6.5" style="13" customWidth="1"/>
-    <col min="4110" max="4110" width="6.33203125" style="13" customWidth="1"/>
-    <col min="4111" max="4111" width="12.5" style="13" customWidth="1"/>
-    <col min="4112" max="4112" width="8.1640625" style="13" customWidth="1"/>
-    <col min="4113" max="4114" width="8.5" style="13" customWidth="1"/>
-    <col min="4115" max="4115" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4116" max="4116" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4117" max="4117" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="10.36328125" style="13" customWidth="1"/>
+    <col min="4105" max="4105" width="9.453125" style="13" customWidth="1"/>
+    <col min="4106" max="4106" width="10.1796875" style="13" customWidth="1"/>
+    <col min="4107" max="4107" width="12.453125" style="13" customWidth="1"/>
+    <col min="4108" max="4108" width="6.6328125" style="13" customWidth="1"/>
+    <col min="4109" max="4109" width="6.453125" style="13" customWidth="1"/>
+    <col min="4110" max="4110" width="6.36328125" style="13" customWidth="1"/>
+    <col min="4111" max="4111" width="12.453125" style="13" customWidth="1"/>
+    <col min="4112" max="4112" width="8.1796875" style="13" customWidth="1"/>
+    <col min="4113" max="4114" width="8.453125" style="13" customWidth="1"/>
+    <col min="4115" max="4115" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4116" max="4116" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4117" max="4117" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="4118" max="4118" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="4119" max="4119" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4119" max="4119" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4120" max="4120" width="18" style="13" customWidth="1"/>
-    <col min="4121" max="4121" width="7.5" style="13" customWidth="1"/>
-    <col min="4122" max="4122" width="10.5" style="13" customWidth="1"/>
-    <col min="4123" max="4352" width="8.83203125" style="13"/>
-    <col min="4353" max="4353" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4121" width="7.453125" style="13" customWidth="1"/>
+    <col min="4122" max="4122" width="10.453125" style="13" customWidth="1"/>
+    <col min="4123" max="4352" width="8.81640625" style="13"/>
+    <col min="4353" max="4353" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4355" max="4355" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="4356" max="4356" width="7.6640625" style="13" customWidth="1"/>
+    <col min="4356" max="4356" width="7.6328125" style="13" customWidth="1"/>
     <col min="4357" max="4357" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="4358" max="4358" width="8" style="13" customWidth="1"/>
     <col min="4359" max="4359" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="10.33203125" style="13" customWidth="1"/>
-    <col min="4361" max="4361" width="9.5" style="13" customWidth="1"/>
-    <col min="4362" max="4362" width="10.1640625" style="13" customWidth="1"/>
-    <col min="4363" max="4363" width="12.5" style="13" customWidth="1"/>
-    <col min="4364" max="4364" width="6.6640625" style="13" customWidth="1"/>
-    <col min="4365" max="4365" width="6.5" style="13" customWidth="1"/>
-    <col min="4366" max="4366" width="6.33203125" style="13" customWidth="1"/>
-    <col min="4367" max="4367" width="12.5" style="13" customWidth="1"/>
-    <col min="4368" max="4368" width="8.1640625" style="13" customWidth="1"/>
-    <col min="4369" max="4370" width="8.5" style="13" customWidth="1"/>
-    <col min="4371" max="4371" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4372" max="4372" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4373" max="4373" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="10.36328125" style="13" customWidth="1"/>
+    <col min="4361" max="4361" width="9.453125" style="13" customWidth="1"/>
+    <col min="4362" max="4362" width="10.1796875" style="13" customWidth="1"/>
+    <col min="4363" max="4363" width="12.453125" style="13" customWidth="1"/>
+    <col min="4364" max="4364" width="6.6328125" style="13" customWidth="1"/>
+    <col min="4365" max="4365" width="6.453125" style="13" customWidth="1"/>
+    <col min="4366" max="4366" width="6.36328125" style="13" customWidth="1"/>
+    <col min="4367" max="4367" width="12.453125" style="13" customWidth="1"/>
+    <col min="4368" max="4368" width="8.1796875" style="13" customWidth="1"/>
+    <col min="4369" max="4370" width="8.453125" style="13" customWidth="1"/>
+    <col min="4371" max="4371" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4372" max="4372" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4373" max="4373" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="4374" max="4374" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="4375" max="4375" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4375" max="4375" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4376" max="4376" width="18" style="13" customWidth="1"/>
-    <col min="4377" max="4377" width="7.5" style="13" customWidth="1"/>
-    <col min="4378" max="4378" width="10.5" style="13" customWidth="1"/>
-    <col min="4379" max="4608" width="8.83203125" style="13"/>
-    <col min="4609" max="4609" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4377" width="7.453125" style="13" customWidth="1"/>
+    <col min="4378" max="4378" width="10.453125" style="13" customWidth="1"/>
+    <col min="4379" max="4608" width="8.81640625" style="13"/>
+    <col min="4609" max="4609" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4611" max="4611" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="4612" max="4612" width="7.6640625" style="13" customWidth="1"/>
+    <col min="4612" max="4612" width="7.6328125" style="13" customWidth="1"/>
     <col min="4613" max="4613" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="4614" max="4614" width="8" style="13" customWidth="1"/>
     <col min="4615" max="4615" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="10.33203125" style="13" customWidth="1"/>
-    <col min="4617" max="4617" width="9.5" style="13" customWidth="1"/>
-    <col min="4618" max="4618" width="10.1640625" style="13" customWidth="1"/>
-    <col min="4619" max="4619" width="12.5" style="13" customWidth="1"/>
-    <col min="4620" max="4620" width="6.6640625" style="13" customWidth="1"/>
-    <col min="4621" max="4621" width="6.5" style="13" customWidth="1"/>
-    <col min="4622" max="4622" width="6.33203125" style="13" customWidth="1"/>
-    <col min="4623" max="4623" width="12.5" style="13" customWidth="1"/>
-    <col min="4624" max="4624" width="8.1640625" style="13" customWidth="1"/>
-    <col min="4625" max="4626" width="8.5" style="13" customWidth="1"/>
-    <col min="4627" max="4627" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4628" max="4628" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4629" max="4629" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="10.36328125" style="13" customWidth="1"/>
+    <col min="4617" max="4617" width="9.453125" style="13" customWidth="1"/>
+    <col min="4618" max="4618" width="10.1796875" style="13" customWidth="1"/>
+    <col min="4619" max="4619" width="12.453125" style="13" customWidth="1"/>
+    <col min="4620" max="4620" width="6.6328125" style="13" customWidth="1"/>
+    <col min="4621" max="4621" width="6.453125" style="13" customWidth="1"/>
+    <col min="4622" max="4622" width="6.36328125" style="13" customWidth="1"/>
+    <col min="4623" max="4623" width="12.453125" style="13" customWidth="1"/>
+    <col min="4624" max="4624" width="8.1796875" style="13" customWidth="1"/>
+    <col min="4625" max="4626" width="8.453125" style="13" customWidth="1"/>
+    <col min="4627" max="4627" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4628" max="4628" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4629" max="4629" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="4630" max="4630" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="4631" max="4631" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4631" max="4631" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4632" max="4632" width="18" style="13" customWidth="1"/>
-    <col min="4633" max="4633" width="7.5" style="13" customWidth="1"/>
-    <col min="4634" max="4634" width="10.5" style="13" customWidth="1"/>
-    <col min="4635" max="4864" width="8.83203125" style="13"/>
-    <col min="4865" max="4865" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4633" width="7.453125" style="13" customWidth="1"/>
+    <col min="4634" max="4634" width="10.453125" style="13" customWidth="1"/>
+    <col min="4635" max="4864" width="8.81640625" style="13"/>
+    <col min="4865" max="4865" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4867" max="4867" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="4868" max="4868" width="7.6640625" style="13" customWidth="1"/>
+    <col min="4868" max="4868" width="7.6328125" style="13" customWidth="1"/>
     <col min="4869" max="4869" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="4870" max="4870" width="8" style="13" customWidth="1"/>
     <col min="4871" max="4871" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="10.33203125" style="13" customWidth="1"/>
-    <col min="4873" max="4873" width="9.5" style="13" customWidth="1"/>
-    <col min="4874" max="4874" width="10.1640625" style="13" customWidth="1"/>
-    <col min="4875" max="4875" width="12.5" style="13" customWidth="1"/>
-    <col min="4876" max="4876" width="6.6640625" style="13" customWidth="1"/>
-    <col min="4877" max="4877" width="6.5" style="13" customWidth="1"/>
-    <col min="4878" max="4878" width="6.33203125" style="13" customWidth="1"/>
-    <col min="4879" max="4879" width="12.5" style="13" customWidth="1"/>
-    <col min="4880" max="4880" width="8.1640625" style="13" customWidth="1"/>
-    <col min="4881" max="4882" width="8.5" style="13" customWidth="1"/>
-    <col min="4883" max="4883" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4884" max="4884" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4885" max="4885" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="10.36328125" style="13" customWidth="1"/>
+    <col min="4873" max="4873" width="9.453125" style="13" customWidth="1"/>
+    <col min="4874" max="4874" width="10.1796875" style="13" customWidth="1"/>
+    <col min="4875" max="4875" width="12.453125" style="13" customWidth="1"/>
+    <col min="4876" max="4876" width="6.6328125" style="13" customWidth="1"/>
+    <col min="4877" max="4877" width="6.453125" style="13" customWidth="1"/>
+    <col min="4878" max="4878" width="6.36328125" style="13" customWidth="1"/>
+    <col min="4879" max="4879" width="12.453125" style="13" customWidth="1"/>
+    <col min="4880" max="4880" width="8.1796875" style="13" customWidth="1"/>
+    <col min="4881" max="4882" width="8.453125" style="13" customWidth="1"/>
+    <col min="4883" max="4883" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4884" max="4884" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4885" max="4885" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="4886" max="4886" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="4887" max="4887" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4887" max="4887" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="4888" max="4888" width="18" style="13" customWidth="1"/>
-    <col min="4889" max="4889" width="7.5" style="13" customWidth="1"/>
-    <col min="4890" max="4890" width="10.5" style="13" customWidth="1"/>
-    <col min="4891" max="5120" width="8.83203125" style="13"/>
-    <col min="5121" max="5121" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4889" max="4889" width="7.453125" style="13" customWidth="1"/>
+    <col min="4890" max="4890" width="10.453125" style="13" customWidth="1"/>
+    <col min="4891" max="5120" width="8.81640625" style="13"/>
+    <col min="5121" max="5121" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5123" max="5123" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="5124" max="5124" width="7.6640625" style="13" customWidth="1"/>
+    <col min="5124" max="5124" width="7.6328125" style="13" customWidth="1"/>
     <col min="5125" max="5125" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="5126" max="5126" width="8" style="13" customWidth="1"/>
     <col min="5127" max="5127" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="10.33203125" style="13" customWidth="1"/>
-    <col min="5129" max="5129" width="9.5" style="13" customWidth="1"/>
-    <col min="5130" max="5130" width="10.1640625" style="13" customWidth="1"/>
-    <col min="5131" max="5131" width="12.5" style="13" customWidth="1"/>
-    <col min="5132" max="5132" width="6.6640625" style="13" customWidth="1"/>
-    <col min="5133" max="5133" width="6.5" style="13" customWidth="1"/>
-    <col min="5134" max="5134" width="6.33203125" style="13" customWidth="1"/>
-    <col min="5135" max="5135" width="12.5" style="13" customWidth="1"/>
-    <col min="5136" max="5136" width="8.1640625" style="13" customWidth="1"/>
-    <col min="5137" max="5138" width="8.5" style="13" customWidth="1"/>
-    <col min="5139" max="5139" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5140" max="5140" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5141" max="5141" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="10.36328125" style="13" customWidth="1"/>
+    <col min="5129" max="5129" width="9.453125" style="13" customWidth="1"/>
+    <col min="5130" max="5130" width="10.1796875" style="13" customWidth="1"/>
+    <col min="5131" max="5131" width="12.453125" style="13" customWidth="1"/>
+    <col min="5132" max="5132" width="6.6328125" style="13" customWidth="1"/>
+    <col min="5133" max="5133" width="6.453125" style="13" customWidth="1"/>
+    <col min="5134" max="5134" width="6.36328125" style="13" customWidth="1"/>
+    <col min="5135" max="5135" width="12.453125" style="13" customWidth="1"/>
+    <col min="5136" max="5136" width="8.1796875" style="13" customWidth="1"/>
+    <col min="5137" max="5138" width="8.453125" style="13" customWidth="1"/>
+    <col min="5139" max="5139" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5140" max="5140" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5141" max="5141" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="5142" max="5142" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="5143" max="5143" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5143" max="5143" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5144" max="5144" width="18" style="13" customWidth="1"/>
-    <col min="5145" max="5145" width="7.5" style="13" customWidth="1"/>
-    <col min="5146" max="5146" width="10.5" style="13" customWidth="1"/>
-    <col min="5147" max="5376" width="8.83203125" style="13"/>
-    <col min="5377" max="5377" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5145" width="7.453125" style="13" customWidth="1"/>
+    <col min="5146" max="5146" width="10.453125" style="13" customWidth="1"/>
+    <col min="5147" max="5376" width="8.81640625" style="13"/>
+    <col min="5377" max="5377" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5379" max="5379" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="5380" max="5380" width="7.6640625" style="13" customWidth="1"/>
+    <col min="5380" max="5380" width="7.6328125" style="13" customWidth="1"/>
     <col min="5381" max="5381" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="5382" max="5382" width="8" style="13" customWidth="1"/>
     <col min="5383" max="5383" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="10.33203125" style="13" customWidth="1"/>
-    <col min="5385" max="5385" width="9.5" style="13" customWidth="1"/>
-    <col min="5386" max="5386" width="10.1640625" style="13" customWidth="1"/>
-    <col min="5387" max="5387" width="12.5" style="13" customWidth="1"/>
-    <col min="5388" max="5388" width="6.6640625" style="13" customWidth="1"/>
-    <col min="5389" max="5389" width="6.5" style="13" customWidth="1"/>
-    <col min="5390" max="5390" width="6.33203125" style="13" customWidth="1"/>
-    <col min="5391" max="5391" width="12.5" style="13" customWidth="1"/>
-    <col min="5392" max="5392" width="8.1640625" style="13" customWidth="1"/>
-    <col min="5393" max="5394" width="8.5" style="13" customWidth="1"/>
-    <col min="5395" max="5395" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5396" max="5396" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5397" max="5397" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="10.36328125" style="13" customWidth="1"/>
+    <col min="5385" max="5385" width="9.453125" style="13" customWidth="1"/>
+    <col min="5386" max="5386" width="10.1796875" style="13" customWidth="1"/>
+    <col min="5387" max="5387" width="12.453125" style="13" customWidth="1"/>
+    <col min="5388" max="5388" width="6.6328125" style="13" customWidth="1"/>
+    <col min="5389" max="5389" width="6.453125" style="13" customWidth="1"/>
+    <col min="5390" max="5390" width="6.36328125" style="13" customWidth="1"/>
+    <col min="5391" max="5391" width="12.453125" style="13" customWidth="1"/>
+    <col min="5392" max="5392" width="8.1796875" style="13" customWidth="1"/>
+    <col min="5393" max="5394" width="8.453125" style="13" customWidth="1"/>
+    <col min="5395" max="5395" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5396" max="5396" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5397" max="5397" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="5398" max="5398" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="5399" max="5399" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5399" max="5399" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5400" max="5400" width="18" style="13" customWidth="1"/>
-    <col min="5401" max="5401" width="7.5" style="13" customWidth="1"/>
-    <col min="5402" max="5402" width="10.5" style="13" customWidth="1"/>
-    <col min="5403" max="5632" width="8.83203125" style="13"/>
-    <col min="5633" max="5633" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5401" width="7.453125" style="13" customWidth="1"/>
+    <col min="5402" max="5402" width="10.453125" style="13" customWidth="1"/>
+    <col min="5403" max="5632" width="8.81640625" style="13"/>
+    <col min="5633" max="5633" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5635" max="5635" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="5636" max="5636" width="7.6640625" style="13" customWidth="1"/>
+    <col min="5636" max="5636" width="7.6328125" style="13" customWidth="1"/>
     <col min="5637" max="5637" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="5638" max="5638" width="8" style="13" customWidth="1"/>
     <col min="5639" max="5639" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="10.33203125" style="13" customWidth="1"/>
-    <col min="5641" max="5641" width="9.5" style="13" customWidth="1"/>
-    <col min="5642" max="5642" width="10.1640625" style="13" customWidth="1"/>
-    <col min="5643" max="5643" width="12.5" style="13" customWidth="1"/>
-    <col min="5644" max="5644" width="6.6640625" style="13" customWidth="1"/>
-    <col min="5645" max="5645" width="6.5" style="13" customWidth="1"/>
-    <col min="5646" max="5646" width="6.33203125" style="13" customWidth="1"/>
-    <col min="5647" max="5647" width="12.5" style="13" customWidth="1"/>
-    <col min="5648" max="5648" width="8.1640625" style="13" customWidth="1"/>
-    <col min="5649" max="5650" width="8.5" style="13" customWidth="1"/>
-    <col min="5651" max="5651" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5652" max="5652" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5653" max="5653" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="10.36328125" style="13" customWidth="1"/>
+    <col min="5641" max="5641" width="9.453125" style="13" customWidth="1"/>
+    <col min="5642" max="5642" width="10.1796875" style="13" customWidth="1"/>
+    <col min="5643" max="5643" width="12.453125" style="13" customWidth="1"/>
+    <col min="5644" max="5644" width="6.6328125" style="13" customWidth="1"/>
+    <col min="5645" max="5645" width="6.453125" style="13" customWidth="1"/>
+    <col min="5646" max="5646" width="6.36328125" style="13" customWidth="1"/>
+    <col min="5647" max="5647" width="12.453125" style="13" customWidth="1"/>
+    <col min="5648" max="5648" width="8.1796875" style="13" customWidth="1"/>
+    <col min="5649" max="5650" width="8.453125" style="13" customWidth="1"/>
+    <col min="5651" max="5651" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5652" max="5652" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5653" max="5653" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="5654" max="5654" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="5655" max="5655" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5655" max="5655" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5656" max="5656" width="18" style="13" customWidth="1"/>
-    <col min="5657" max="5657" width="7.5" style="13" customWidth="1"/>
-    <col min="5658" max="5658" width="10.5" style="13" customWidth="1"/>
-    <col min="5659" max="5888" width="8.83203125" style="13"/>
-    <col min="5889" max="5889" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5657" width="7.453125" style="13" customWidth="1"/>
+    <col min="5658" max="5658" width="10.453125" style="13" customWidth="1"/>
+    <col min="5659" max="5888" width="8.81640625" style="13"/>
+    <col min="5889" max="5889" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5891" max="5891" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="5892" max="5892" width="7.6640625" style="13" customWidth="1"/>
+    <col min="5892" max="5892" width="7.6328125" style="13" customWidth="1"/>
     <col min="5893" max="5893" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="5894" max="5894" width="8" style="13" customWidth="1"/>
     <col min="5895" max="5895" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="10.33203125" style="13" customWidth="1"/>
-    <col min="5897" max="5897" width="9.5" style="13" customWidth="1"/>
-    <col min="5898" max="5898" width="10.1640625" style="13" customWidth="1"/>
-    <col min="5899" max="5899" width="12.5" style="13" customWidth="1"/>
-    <col min="5900" max="5900" width="6.6640625" style="13" customWidth="1"/>
-    <col min="5901" max="5901" width="6.5" style="13" customWidth="1"/>
-    <col min="5902" max="5902" width="6.33203125" style="13" customWidth="1"/>
-    <col min="5903" max="5903" width="12.5" style="13" customWidth="1"/>
-    <col min="5904" max="5904" width="8.1640625" style="13" customWidth="1"/>
-    <col min="5905" max="5906" width="8.5" style="13" customWidth="1"/>
-    <col min="5907" max="5907" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5908" max="5908" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5909" max="5909" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="10.36328125" style="13" customWidth="1"/>
+    <col min="5897" max="5897" width="9.453125" style="13" customWidth="1"/>
+    <col min="5898" max="5898" width="10.1796875" style="13" customWidth="1"/>
+    <col min="5899" max="5899" width="12.453125" style="13" customWidth="1"/>
+    <col min="5900" max="5900" width="6.6328125" style="13" customWidth="1"/>
+    <col min="5901" max="5901" width="6.453125" style="13" customWidth="1"/>
+    <col min="5902" max="5902" width="6.36328125" style="13" customWidth="1"/>
+    <col min="5903" max="5903" width="12.453125" style="13" customWidth="1"/>
+    <col min="5904" max="5904" width="8.1796875" style="13" customWidth="1"/>
+    <col min="5905" max="5906" width="8.453125" style="13" customWidth="1"/>
+    <col min="5907" max="5907" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5908" max="5908" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5909" max="5909" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="5910" max="5910" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="5911" max="5911" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5911" max="5911" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="5912" max="5912" width="18" style="13" customWidth="1"/>
-    <col min="5913" max="5913" width="7.5" style="13" customWidth="1"/>
-    <col min="5914" max="5914" width="10.5" style="13" customWidth="1"/>
-    <col min="5915" max="6144" width="8.83203125" style="13"/>
-    <col min="6145" max="6145" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5913" max="5913" width="7.453125" style="13" customWidth="1"/>
+    <col min="5914" max="5914" width="10.453125" style="13" customWidth="1"/>
+    <col min="5915" max="6144" width="8.81640625" style="13"/>
+    <col min="6145" max="6145" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6147" max="6147" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="6148" max="6148" width="7.6640625" style="13" customWidth="1"/>
+    <col min="6148" max="6148" width="7.6328125" style="13" customWidth="1"/>
     <col min="6149" max="6149" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="6150" max="6150" width="8" style="13" customWidth="1"/>
     <col min="6151" max="6151" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="10.33203125" style="13" customWidth="1"/>
-    <col min="6153" max="6153" width="9.5" style="13" customWidth="1"/>
-    <col min="6154" max="6154" width="10.1640625" style="13" customWidth="1"/>
-    <col min="6155" max="6155" width="12.5" style="13" customWidth="1"/>
-    <col min="6156" max="6156" width="6.6640625" style="13" customWidth="1"/>
-    <col min="6157" max="6157" width="6.5" style="13" customWidth="1"/>
-    <col min="6158" max="6158" width="6.33203125" style="13" customWidth="1"/>
-    <col min="6159" max="6159" width="12.5" style="13" customWidth="1"/>
-    <col min="6160" max="6160" width="8.1640625" style="13" customWidth="1"/>
-    <col min="6161" max="6162" width="8.5" style="13" customWidth="1"/>
-    <col min="6163" max="6163" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6164" max="6164" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6165" max="6165" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="10.36328125" style="13" customWidth="1"/>
+    <col min="6153" max="6153" width="9.453125" style="13" customWidth="1"/>
+    <col min="6154" max="6154" width="10.1796875" style="13" customWidth="1"/>
+    <col min="6155" max="6155" width="12.453125" style="13" customWidth="1"/>
+    <col min="6156" max="6156" width="6.6328125" style="13" customWidth="1"/>
+    <col min="6157" max="6157" width="6.453125" style="13" customWidth="1"/>
+    <col min="6158" max="6158" width="6.36328125" style="13" customWidth="1"/>
+    <col min="6159" max="6159" width="12.453125" style="13" customWidth="1"/>
+    <col min="6160" max="6160" width="8.1796875" style="13" customWidth="1"/>
+    <col min="6161" max="6162" width="8.453125" style="13" customWidth="1"/>
+    <col min="6163" max="6163" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6164" max="6164" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6165" max="6165" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="6166" max="6166" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="6167" max="6167" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6167" max="6167" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6168" max="6168" width="18" style="13" customWidth="1"/>
-    <col min="6169" max="6169" width="7.5" style="13" customWidth="1"/>
-    <col min="6170" max="6170" width="10.5" style="13" customWidth="1"/>
-    <col min="6171" max="6400" width="8.83203125" style="13"/>
-    <col min="6401" max="6401" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6169" width="7.453125" style="13" customWidth="1"/>
+    <col min="6170" max="6170" width="10.453125" style="13" customWidth="1"/>
+    <col min="6171" max="6400" width="8.81640625" style="13"/>
+    <col min="6401" max="6401" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6403" max="6403" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="6404" max="6404" width="7.6640625" style="13" customWidth="1"/>
+    <col min="6404" max="6404" width="7.6328125" style="13" customWidth="1"/>
     <col min="6405" max="6405" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="6406" max="6406" width="8" style="13" customWidth="1"/>
     <col min="6407" max="6407" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="10.33203125" style="13" customWidth="1"/>
-    <col min="6409" max="6409" width="9.5" style="13" customWidth="1"/>
-    <col min="6410" max="6410" width="10.1640625" style="13" customWidth="1"/>
-    <col min="6411" max="6411" width="12.5" style="13" customWidth="1"/>
-    <col min="6412" max="6412" width="6.6640625" style="13" customWidth="1"/>
-    <col min="6413" max="6413" width="6.5" style="13" customWidth="1"/>
-    <col min="6414" max="6414" width="6.33203125" style="13" customWidth="1"/>
-    <col min="6415" max="6415" width="12.5" style="13" customWidth="1"/>
-    <col min="6416" max="6416" width="8.1640625" style="13" customWidth="1"/>
-    <col min="6417" max="6418" width="8.5" style="13" customWidth="1"/>
-    <col min="6419" max="6419" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6420" max="6420" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6421" max="6421" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="10.36328125" style="13" customWidth="1"/>
+    <col min="6409" max="6409" width="9.453125" style="13" customWidth="1"/>
+    <col min="6410" max="6410" width="10.1796875" style="13" customWidth="1"/>
+    <col min="6411" max="6411" width="12.453125" style="13" customWidth="1"/>
+    <col min="6412" max="6412" width="6.6328125" style="13" customWidth="1"/>
+    <col min="6413" max="6413" width="6.453125" style="13" customWidth="1"/>
+    <col min="6414" max="6414" width="6.36328125" style="13" customWidth="1"/>
+    <col min="6415" max="6415" width="12.453125" style="13" customWidth="1"/>
+    <col min="6416" max="6416" width="8.1796875" style="13" customWidth="1"/>
+    <col min="6417" max="6418" width="8.453125" style="13" customWidth="1"/>
+    <col min="6419" max="6419" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6420" max="6420" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6421" max="6421" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="6422" max="6422" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="6423" max="6423" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6423" max="6423" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6424" max="6424" width="18" style="13" customWidth="1"/>
-    <col min="6425" max="6425" width="7.5" style="13" customWidth="1"/>
-    <col min="6426" max="6426" width="10.5" style="13" customWidth="1"/>
-    <col min="6427" max="6656" width="8.83203125" style="13"/>
-    <col min="6657" max="6657" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6425" width="7.453125" style="13" customWidth="1"/>
+    <col min="6426" max="6426" width="10.453125" style="13" customWidth="1"/>
+    <col min="6427" max="6656" width="8.81640625" style="13"/>
+    <col min="6657" max="6657" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6659" max="6659" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="6660" max="6660" width="7.6640625" style="13" customWidth="1"/>
+    <col min="6660" max="6660" width="7.6328125" style="13" customWidth="1"/>
     <col min="6661" max="6661" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="6662" max="6662" width="8" style="13" customWidth="1"/>
     <col min="6663" max="6663" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="10.33203125" style="13" customWidth="1"/>
-    <col min="6665" max="6665" width="9.5" style="13" customWidth="1"/>
-    <col min="6666" max="6666" width="10.1640625" style="13" customWidth="1"/>
-    <col min="6667" max="6667" width="12.5" style="13" customWidth="1"/>
-    <col min="6668" max="6668" width="6.6640625" style="13" customWidth="1"/>
-    <col min="6669" max="6669" width="6.5" style="13" customWidth="1"/>
-    <col min="6670" max="6670" width="6.33203125" style="13" customWidth="1"/>
-    <col min="6671" max="6671" width="12.5" style="13" customWidth="1"/>
-    <col min="6672" max="6672" width="8.1640625" style="13" customWidth="1"/>
-    <col min="6673" max="6674" width="8.5" style="13" customWidth="1"/>
-    <col min="6675" max="6675" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6676" max="6676" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6677" max="6677" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="10.36328125" style="13" customWidth="1"/>
+    <col min="6665" max="6665" width="9.453125" style="13" customWidth="1"/>
+    <col min="6666" max="6666" width="10.1796875" style="13" customWidth="1"/>
+    <col min="6667" max="6667" width="12.453125" style="13" customWidth="1"/>
+    <col min="6668" max="6668" width="6.6328125" style="13" customWidth="1"/>
+    <col min="6669" max="6669" width="6.453125" style="13" customWidth="1"/>
+    <col min="6670" max="6670" width="6.36328125" style="13" customWidth="1"/>
+    <col min="6671" max="6671" width="12.453125" style="13" customWidth="1"/>
+    <col min="6672" max="6672" width="8.1796875" style="13" customWidth="1"/>
+    <col min="6673" max="6674" width="8.453125" style="13" customWidth="1"/>
+    <col min="6675" max="6675" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6676" max="6676" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6677" max="6677" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="6678" max="6678" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="6679" max="6679" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6679" max="6679" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6680" max="6680" width="18" style="13" customWidth="1"/>
-    <col min="6681" max="6681" width="7.5" style="13" customWidth="1"/>
-    <col min="6682" max="6682" width="10.5" style="13" customWidth="1"/>
-    <col min="6683" max="6912" width="8.83203125" style="13"/>
-    <col min="6913" max="6913" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6681" width="7.453125" style="13" customWidth="1"/>
+    <col min="6682" max="6682" width="10.453125" style="13" customWidth="1"/>
+    <col min="6683" max="6912" width="8.81640625" style="13"/>
+    <col min="6913" max="6913" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6915" max="6915" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="6916" max="6916" width="7.6640625" style="13" customWidth="1"/>
+    <col min="6916" max="6916" width="7.6328125" style="13" customWidth="1"/>
     <col min="6917" max="6917" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="6918" max="6918" width="8" style="13" customWidth="1"/>
     <col min="6919" max="6919" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="10.33203125" style="13" customWidth="1"/>
-    <col min="6921" max="6921" width="9.5" style="13" customWidth="1"/>
-    <col min="6922" max="6922" width="10.1640625" style="13" customWidth="1"/>
-    <col min="6923" max="6923" width="12.5" style="13" customWidth="1"/>
-    <col min="6924" max="6924" width="6.6640625" style="13" customWidth="1"/>
-    <col min="6925" max="6925" width="6.5" style="13" customWidth="1"/>
-    <col min="6926" max="6926" width="6.33203125" style="13" customWidth="1"/>
-    <col min="6927" max="6927" width="12.5" style="13" customWidth="1"/>
-    <col min="6928" max="6928" width="8.1640625" style="13" customWidth="1"/>
-    <col min="6929" max="6930" width="8.5" style="13" customWidth="1"/>
-    <col min="6931" max="6931" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6932" max="6932" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6933" max="6933" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="10.36328125" style="13" customWidth="1"/>
+    <col min="6921" max="6921" width="9.453125" style="13" customWidth="1"/>
+    <col min="6922" max="6922" width="10.1796875" style="13" customWidth="1"/>
+    <col min="6923" max="6923" width="12.453125" style="13" customWidth="1"/>
+    <col min="6924" max="6924" width="6.6328125" style="13" customWidth="1"/>
+    <col min="6925" max="6925" width="6.453125" style="13" customWidth="1"/>
+    <col min="6926" max="6926" width="6.36328125" style="13" customWidth="1"/>
+    <col min="6927" max="6927" width="12.453125" style="13" customWidth="1"/>
+    <col min="6928" max="6928" width="8.1796875" style="13" customWidth="1"/>
+    <col min="6929" max="6930" width="8.453125" style="13" customWidth="1"/>
+    <col min="6931" max="6931" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6932" max="6932" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6933" max="6933" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="6934" max="6934" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="6935" max="6935" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6935" max="6935" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="6936" max="6936" width="18" style="13" customWidth="1"/>
-    <col min="6937" max="6937" width="7.5" style="13" customWidth="1"/>
-    <col min="6938" max="6938" width="10.5" style="13" customWidth="1"/>
-    <col min="6939" max="7168" width="8.83203125" style="13"/>
-    <col min="7169" max="7169" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6937" max="6937" width="7.453125" style="13" customWidth="1"/>
+    <col min="6938" max="6938" width="10.453125" style="13" customWidth="1"/>
+    <col min="6939" max="7168" width="8.81640625" style="13"/>
+    <col min="7169" max="7169" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7171" max="7171" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="7172" max="7172" width="7.6640625" style="13" customWidth="1"/>
+    <col min="7172" max="7172" width="7.6328125" style="13" customWidth="1"/>
     <col min="7173" max="7173" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="7174" max="7174" width="8" style="13" customWidth="1"/>
     <col min="7175" max="7175" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="10.33203125" style="13" customWidth="1"/>
-    <col min="7177" max="7177" width="9.5" style="13" customWidth="1"/>
-    <col min="7178" max="7178" width="10.1640625" style="13" customWidth="1"/>
-    <col min="7179" max="7179" width="12.5" style="13" customWidth="1"/>
-    <col min="7180" max="7180" width="6.6640625" style="13" customWidth="1"/>
-    <col min="7181" max="7181" width="6.5" style="13" customWidth="1"/>
-    <col min="7182" max="7182" width="6.33203125" style="13" customWidth="1"/>
-    <col min="7183" max="7183" width="12.5" style="13" customWidth="1"/>
-    <col min="7184" max="7184" width="8.1640625" style="13" customWidth="1"/>
-    <col min="7185" max="7186" width="8.5" style="13" customWidth="1"/>
-    <col min="7187" max="7187" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7188" max="7188" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7189" max="7189" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="10.36328125" style="13" customWidth="1"/>
+    <col min="7177" max="7177" width="9.453125" style="13" customWidth="1"/>
+    <col min="7178" max="7178" width="10.1796875" style="13" customWidth="1"/>
+    <col min="7179" max="7179" width="12.453125" style="13" customWidth="1"/>
+    <col min="7180" max="7180" width="6.6328125" style="13" customWidth="1"/>
+    <col min="7181" max="7181" width="6.453125" style="13" customWidth="1"/>
+    <col min="7182" max="7182" width="6.36328125" style="13" customWidth="1"/>
+    <col min="7183" max="7183" width="12.453125" style="13" customWidth="1"/>
+    <col min="7184" max="7184" width="8.1796875" style="13" customWidth="1"/>
+    <col min="7185" max="7186" width="8.453125" style="13" customWidth="1"/>
+    <col min="7187" max="7187" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7188" max="7188" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7189" max="7189" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="7190" max="7190" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="7191" max="7191" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7191" max="7191" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7192" max="7192" width="18" style="13" customWidth="1"/>
-    <col min="7193" max="7193" width="7.5" style="13" customWidth="1"/>
-    <col min="7194" max="7194" width="10.5" style="13" customWidth="1"/>
-    <col min="7195" max="7424" width="8.83203125" style="13"/>
-    <col min="7425" max="7425" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7193" width="7.453125" style="13" customWidth="1"/>
+    <col min="7194" max="7194" width="10.453125" style="13" customWidth="1"/>
+    <col min="7195" max="7424" width="8.81640625" style="13"/>
+    <col min="7425" max="7425" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7427" max="7427" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="7428" max="7428" width="7.6640625" style="13" customWidth="1"/>
+    <col min="7428" max="7428" width="7.6328125" style="13" customWidth="1"/>
     <col min="7429" max="7429" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="7430" max="7430" width="8" style="13" customWidth="1"/>
     <col min="7431" max="7431" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="10.33203125" style="13" customWidth="1"/>
-    <col min="7433" max="7433" width="9.5" style="13" customWidth="1"/>
-    <col min="7434" max="7434" width="10.1640625" style="13" customWidth="1"/>
-    <col min="7435" max="7435" width="12.5" style="13" customWidth="1"/>
-    <col min="7436" max="7436" width="6.6640625" style="13" customWidth="1"/>
-    <col min="7437" max="7437" width="6.5" style="13" customWidth="1"/>
-    <col min="7438" max="7438" width="6.33203125" style="13" customWidth="1"/>
-    <col min="7439" max="7439" width="12.5" style="13" customWidth="1"/>
-    <col min="7440" max="7440" width="8.1640625" style="13" customWidth="1"/>
-    <col min="7441" max="7442" width="8.5" style="13" customWidth="1"/>
-    <col min="7443" max="7443" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7444" max="7444" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7445" max="7445" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="10.36328125" style="13" customWidth="1"/>
+    <col min="7433" max="7433" width="9.453125" style="13" customWidth="1"/>
+    <col min="7434" max="7434" width="10.1796875" style="13" customWidth="1"/>
+    <col min="7435" max="7435" width="12.453125" style="13" customWidth="1"/>
+    <col min="7436" max="7436" width="6.6328125" style="13" customWidth="1"/>
+    <col min="7437" max="7437" width="6.453125" style="13" customWidth="1"/>
+    <col min="7438" max="7438" width="6.36328125" style="13" customWidth="1"/>
+    <col min="7439" max="7439" width="12.453125" style="13" customWidth="1"/>
+    <col min="7440" max="7440" width="8.1796875" style="13" customWidth="1"/>
+    <col min="7441" max="7442" width="8.453125" style="13" customWidth="1"/>
+    <col min="7443" max="7443" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7444" max="7444" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7445" max="7445" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="7446" max="7446" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="7447" max="7447" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7447" max="7447" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7448" max="7448" width="18" style="13" customWidth="1"/>
-    <col min="7449" max="7449" width="7.5" style="13" customWidth="1"/>
-    <col min="7450" max="7450" width="10.5" style="13" customWidth="1"/>
-    <col min="7451" max="7680" width="8.83203125" style="13"/>
-    <col min="7681" max="7681" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7449" width="7.453125" style="13" customWidth="1"/>
+    <col min="7450" max="7450" width="10.453125" style="13" customWidth="1"/>
+    <col min="7451" max="7680" width="8.81640625" style="13"/>
+    <col min="7681" max="7681" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7683" max="7683" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="7684" max="7684" width="7.6640625" style="13" customWidth="1"/>
+    <col min="7684" max="7684" width="7.6328125" style="13" customWidth="1"/>
     <col min="7685" max="7685" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="7686" max="7686" width="8" style="13" customWidth="1"/>
     <col min="7687" max="7687" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="10.33203125" style="13" customWidth="1"/>
-    <col min="7689" max="7689" width="9.5" style="13" customWidth="1"/>
-    <col min="7690" max="7690" width="10.1640625" style="13" customWidth="1"/>
-    <col min="7691" max="7691" width="12.5" style="13" customWidth="1"/>
-    <col min="7692" max="7692" width="6.6640625" style="13" customWidth="1"/>
-    <col min="7693" max="7693" width="6.5" style="13" customWidth="1"/>
-    <col min="7694" max="7694" width="6.33203125" style="13" customWidth="1"/>
-    <col min="7695" max="7695" width="12.5" style="13" customWidth="1"/>
-    <col min="7696" max="7696" width="8.1640625" style="13" customWidth="1"/>
-    <col min="7697" max="7698" width="8.5" style="13" customWidth="1"/>
-    <col min="7699" max="7699" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7700" max="7700" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7701" max="7701" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="10.36328125" style="13" customWidth="1"/>
+    <col min="7689" max="7689" width="9.453125" style="13" customWidth="1"/>
+    <col min="7690" max="7690" width="10.1796875" style="13" customWidth="1"/>
+    <col min="7691" max="7691" width="12.453125" style="13" customWidth="1"/>
+    <col min="7692" max="7692" width="6.6328125" style="13" customWidth="1"/>
+    <col min="7693" max="7693" width="6.453125" style="13" customWidth="1"/>
+    <col min="7694" max="7694" width="6.36328125" style="13" customWidth="1"/>
+    <col min="7695" max="7695" width="12.453125" style="13" customWidth="1"/>
+    <col min="7696" max="7696" width="8.1796875" style="13" customWidth="1"/>
+    <col min="7697" max="7698" width="8.453125" style="13" customWidth="1"/>
+    <col min="7699" max="7699" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7700" max="7700" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7701" max="7701" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="7702" max="7702" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="7703" max="7703" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7703" max="7703" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7704" max="7704" width="18" style="13" customWidth="1"/>
-    <col min="7705" max="7705" width="7.5" style="13" customWidth="1"/>
-    <col min="7706" max="7706" width="10.5" style="13" customWidth="1"/>
-    <col min="7707" max="7936" width="8.83203125" style="13"/>
-    <col min="7937" max="7937" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7705" width="7.453125" style="13" customWidth="1"/>
+    <col min="7706" max="7706" width="10.453125" style="13" customWidth="1"/>
+    <col min="7707" max="7936" width="8.81640625" style="13"/>
+    <col min="7937" max="7937" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7939" max="7939" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="7940" max="7940" width="7.6640625" style="13" customWidth="1"/>
+    <col min="7940" max="7940" width="7.6328125" style="13" customWidth="1"/>
     <col min="7941" max="7941" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="7942" max="7942" width="8" style="13" customWidth="1"/>
     <col min="7943" max="7943" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="10.33203125" style="13" customWidth="1"/>
-    <col min="7945" max="7945" width="9.5" style="13" customWidth="1"/>
-    <col min="7946" max="7946" width="10.1640625" style="13" customWidth="1"/>
-    <col min="7947" max="7947" width="12.5" style="13" customWidth="1"/>
-    <col min="7948" max="7948" width="6.6640625" style="13" customWidth="1"/>
-    <col min="7949" max="7949" width="6.5" style="13" customWidth="1"/>
-    <col min="7950" max="7950" width="6.33203125" style="13" customWidth="1"/>
-    <col min="7951" max="7951" width="12.5" style="13" customWidth="1"/>
-    <col min="7952" max="7952" width="8.1640625" style="13" customWidth="1"/>
-    <col min="7953" max="7954" width="8.5" style="13" customWidth="1"/>
-    <col min="7955" max="7955" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7956" max="7956" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7957" max="7957" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="10.36328125" style="13" customWidth="1"/>
+    <col min="7945" max="7945" width="9.453125" style="13" customWidth="1"/>
+    <col min="7946" max="7946" width="10.1796875" style="13" customWidth="1"/>
+    <col min="7947" max="7947" width="12.453125" style="13" customWidth="1"/>
+    <col min="7948" max="7948" width="6.6328125" style="13" customWidth="1"/>
+    <col min="7949" max="7949" width="6.453125" style="13" customWidth="1"/>
+    <col min="7950" max="7950" width="6.36328125" style="13" customWidth="1"/>
+    <col min="7951" max="7951" width="12.453125" style="13" customWidth="1"/>
+    <col min="7952" max="7952" width="8.1796875" style="13" customWidth="1"/>
+    <col min="7953" max="7954" width="8.453125" style="13" customWidth="1"/>
+    <col min="7955" max="7955" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7956" max="7956" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7957" max="7957" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="7958" max="7958" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="7959" max="7959" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7959" max="7959" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="7960" max="7960" width="18" style="13" customWidth="1"/>
-    <col min="7961" max="7961" width="7.5" style="13" customWidth="1"/>
-    <col min="7962" max="7962" width="10.5" style="13" customWidth="1"/>
-    <col min="7963" max="8192" width="8.83203125" style="13"/>
-    <col min="8193" max="8193" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7961" max="7961" width="7.453125" style="13" customWidth="1"/>
+    <col min="7962" max="7962" width="10.453125" style="13" customWidth="1"/>
+    <col min="7963" max="8192" width="8.81640625" style="13"/>
+    <col min="8193" max="8193" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8195" max="8195" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="8196" max="8196" width="7.6640625" style="13" customWidth="1"/>
+    <col min="8196" max="8196" width="7.6328125" style="13" customWidth="1"/>
     <col min="8197" max="8197" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="8198" max="8198" width="8" style="13" customWidth="1"/>
     <col min="8199" max="8199" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="10.33203125" style="13" customWidth="1"/>
-    <col min="8201" max="8201" width="9.5" style="13" customWidth="1"/>
-    <col min="8202" max="8202" width="10.1640625" style="13" customWidth="1"/>
-    <col min="8203" max="8203" width="12.5" style="13" customWidth="1"/>
-    <col min="8204" max="8204" width="6.6640625" style="13" customWidth="1"/>
-    <col min="8205" max="8205" width="6.5" style="13" customWidth="1"/>
-    <col min="8206" max="8206" width="6.33203125" style="13" customWidth="1"/>
-    <col min="8207" max="8207" width="12.5" style="13" customWidth="1"/>
-    <col min="8208" max="8208" width="8.1640625" style="13" customWidth="1"/>
-    <col min="8209" max="8210" width="8.5" style="13" customWidth="1"/>
-    <col min="8211" max="8211" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8212" max="8212" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8213" max="8213" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="10.36328125" style="13" customWidth="1"/>
+    <col min="8201" max="8201" width="9.453125" style="13" customWidth="1"/>
+    <col min="8202" max="8202" width="10.1796875" style="13" customWidth="1"/>
+    <col min="8203" max="8203" width="12.453125" style="13" customWidth="1"/>
+    <col min="8204" max="8204" width="6.6328125" style="13" customWidth="1"/>
+    <col min="8205" max="8205" width="6.453125" style="13" customWidth="1"/>
+    <col min="8206" max="8206" width="6.36328125" style="13" customWidth="1"/>
+    <col min="8207" max="8207" width="12.453125" style="13" customWidth="1"/>
+    <col min="8208" max="8208" width="8.1796875" style="13" customWidth="1"/>
+    <col min="8209" max="8210" width="8.453125" style="13" customWidth="1"/>
+    <col min="8211" max="8211" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8212" max="8212" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8213" max="8213" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="8214" max="8214" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="8215" max="8215" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8215" max="8215" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8216" max="8216" width="18" style="13" customWidth="1"/>
-    <col min="8217" max="8217" width="7.5" style="13" customWidth="1"/>
-    <col min="8218" max="8218" width="10.5" style="13" customWidth="1"/>
-    <col min="8219" max="8448" width="8.83203125" style="13"/>
-    <col min="8449" max="8449" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8217" width="7.453125" style="13" customWidth="1"/>
+    <col min="8218" max="8218" width="10.453125" style="13" customWidth="1"/>
+    <col min="8219" max="8448" width="8.81640625" style="13"/>
+    <col min="8449" max="8449" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8451" max="8451" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="8452" max="8452" width="7.6640625" style="13" customWidth="1"/>
+    <col min="8452" max="8452" width="7.6328125" style="13" customWidth="1"/>
     <col min="8453" max="8453" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="8454" max="8454" width="8" style="13" customWidth="1"/>
     <col min="8455" max="8455" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="10.33203125" style="13" customWidth="1"/>
-    <col min="8457" max="8457" width="9.5" style="13" customWidth="1"/>
-    <col min="8458" max="8458" width="10.1640625" style="13" customWidth="1"/>
-    <col min="8459" max="8459" width="12.5" style="13" customWidth="1"/>
-    <col min="8460" max="8460" width="6.6640625" style="13" customWidth="1"/>
-    <col min="8461" max="8461" width="6.5" style="13" customWidth="1"/>
-    <col min="8462" max="8462" width="6.33203125" style="13" customWidth="1"/>
-    <col min="8463" max="8463" width="12.5" style="13" customWidth="1"/>
-    <col min="8464" max="8464" width="8.1640625" style="13" customWidth="1"/>
-    <col min="8465" max="8466" width="8.5" style="13" customWidth="1"/>
-    <col min="8467" max="8467" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8468" max="8468" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8469" max="8469" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="10.36328125" style="13" customWidth="1"/>
+    <col min="8457" max="8457" width="9.453125" style="13" customWidth="1"/>
+    <col min="8458" max="8458" width="10.1796875" style="13" customWidth="1"/>
+    <col min="8459" max="8459" width="12.453125" style="13" customWidth="1"/>
+    <col min="8460" max="8460" width="6.6328125" style="13" customWidth="1"/>
+    <col min="8461" max="8461" width="6.453125" style="13" customWidth="1"/>
+    <col min="8462" max="8462" width="6.36328125" style="13" customWidth="1"/>
+    <col min="8463" max="8463" width="12.453125" style="13" customWidth="1"/>
+    <col min="8464" max="8464" width="8.1796875" style="13" customWidth="1"/>
+    <col min="8465" max="8466" width="8.453125" style="13" customWidth="1"/>
+    <col min="8467" max="8467" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8468" max="8468" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8469" max="8469" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="8470" max="8470" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="8471" max="8471" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8471" max="8471" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8472" max="8472" width="18" style="13" customWidth="1"/>
-    <col min="8473" max="8473" width="7.5" style="13" customWidth="1"/>
-    <col min="8474" max="8474" width="10.5" style="13" customWidth="1"/>
-    <col min="8475" max="8704" width="8.83203125" style="13"/>
-    <col min="8705" max="8705" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8473" width="7.453125" style="13" customWidth="1"/>
+    <col min="8474" max="8474" width="10.453125" style="13" customWidth="1"/>
+    <col min="8475" max="8704" width="8.81640625" style="13"/>
+    <col min="8705" max="8705" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8707" max="8707" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="8708" max="8708" width="7.6640625" style="13" customWidth="1"/>
+    <col min="8708" max="8708" width="7.6328125" style="13" customWidth="1"/>
     <col min="8709" max="8709" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="8710" max="8710" width="8" style="13" customWidth="1"/>
     <col min="8711" max="8711" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="10.33203125" style="13" customWidth="1"/>
-    <col min="8713" max="8713" width="9.5" style="13" customWidth="1"/>
-    <col min="8714" max="8714" width="10.1640625" style="13" customWidth="1"/>
-    <col min="8715" max="8715" width="12.5" style="13" customWidth="1"/>
-    <col min="8716" max="8716" width="6.6640625" style="13" customWidth="1"/>
-    <col min="8717" max="8717" width="6.5" style="13" customWidth="1"/>
-    <col min="8718" max="8718" width="6.33203125" style="13" customWidth="1"/>
-    <col min="8719" max="8719" width="12.5" style="13" customWidth="1"/>
-    <col min="8720" max="8720" width="8.1640625" style="13" customWidth="1"/>
-    <col min="8721" max="8722" width="8.5" style="13" customWidth="1"/>
-    <col min="8723" max="8723" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8724" max="8724" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8725" max="8725" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="10.36328125" style="13" customWidth="1"/>
+    <col min="8713" max="8713" width="9.453125" style="13" customWidth="1"/>
+    <col min="8714" max="8714" width="10.1796875" style="13" customWidth="1"/>
+    <col min="8715" max="8715" width="12.453125" style="13" customWidth="1"/>
+    <col min="8716" max="8716" width="6.6328125" style="13" customWidth="1"/>
+    <col min="8717" max="8717" width="6.453125" style="13" customWidth="1"/>
+    <col min="8718" max="8718" width="6.36328125" style="13" customWidth="1"/>
+    <col min="8719" max="8719" width="12.453125" style="13" customWidth="1"/>
+    <col min="8720" max="8720" width="8.1796875" style="13" customWidth="1"/>
+    <col min="8721" max="8722" width="8.453125" style="13" customWidth="1"/>
+    <col min="8723" max="8723" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8724" max="8724" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8725" max="8725" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="8726" max="8726" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="8727" max="8727" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8727" max="8727" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8728" max="8728" width="18" style="13" customWidth="1"/>
-    <col min="8729" max="8729" width="7.5" style="13" customWidth="1"/>
-    <col min="8730" max="8730" width="10.5" style="13" customWidth="1"/>
-    <col min="8731" max="8960" width="8.83203125" style="13"/>
-    <col min="8961" max="8961" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8729" width="7.453125" style="13" customWidth="1"/>
+    <col min="8730" max="8730" width="10.453125" style="13" customWidth="1"/>
+    <col min="8731" max="8960" width="8.81640625" style="13"/>
+    <col min="8961" max="8961" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8963" max="8963" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="8964" max="8964" width="7.6640625" style="13" customWidth="1"/>
+    <col min="8964" max="8964" width="7.6328125" style="13" customWidth="1"/>
     <col min="8965" max="8965" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="8966" max="8966" width="8" style="13" customWidth="1"/>
     <col min="8967" max="8967" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="10.33203125" style="13" customWidth="1"/>
-    <col min="8969" max="8969" width="9.5" style="13" customWidth="1"/>
-    <col min="8970" max="8970" width="10.1640625" style="13" customWidth="1"/>
-    <col min="8971" max="8971" width="12.5" style="13" customWidth="1"/>
-    <col min="8972" max="8972" width="6.6640625" style="13" customWidth="1"/>
-    <col min="8973" max="8973" width="6.5" style="13" customWidth="1"/>
-    <col min="8974" max="8974" width="6.33203125" style="13" customWidth="1"/>
-    <col min="8975" max="8975" width="12.5" style="13" customWidth="1"/>
-    <col min="8976" max="8976" width="8.1640625" style="13" customWidth="1"/>
-    <col min="8977" max="8978" width="8.5" style="13" customWidth="1"/>
-    <col min="8979" max="8979" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8980" max="8980" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8981" max="8981" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="10.36328125" style="13" customWidth="1"/>
+    <col min="8969" max="8969" width="9.453125" style="13" customWidth="1"/>
+    <col min="8970" max="8970" width="10.1796875" style="13" customWidth="1"/>
+    <col min="8971" max="8971" width="12.453125" style="13" customWidth="1"/>
+    <col min="8972" max="8972" width="6.6328125" style="13" customWidth="1"/>
+    <col min="8973" max="8973" width="6.453125" style="13" customWidth="1"/>
+    <col min="8974" max="8974" width="6.36328125" style="13" customWidth="1"/>
+    <col min="8975" max="8975" width="12.453125" style="13" customWidth="1"/>
+    <col min="8976" max="8976" width="8.1796875" style="13" customWidth="1"/>
+    <col min="8977" max="8978" width="8.453125" style="13" customWidth="1"/>
+    <col min="8979" max="8979" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8980" max="8980" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8981" max="8981" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="8982" max="8982" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="8983" max="8983" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8983" max="8983" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="8984" max="8984" width="18" style="13" customWidth="1"/>
-    <col min="8985" max="8985" width="7.5" style="13" customWidth="1"/>
-    <col min="8986" max="8986" width="10.5" style="13" customWidth="1"/>
-    <col min="8987" max="9216" width="8.83203125" style="13"/>
-    <col min="9217" max="9217" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8985" max="8985" width="7.453125" style="13" customWidth="1"/>
+    <col min="8986" max="8986" width="10.453125" style="13" customWidth="1"/>
+    <col min="8987" max="9216" width="8.81640625" style="13"/>
+    <col min="9217" max="9217" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="9219" max="9219" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="9220" max="9220" width="7.6640625" style="13" customWidth="1"/>
+    <col min="9220" max="9220" width="7.6328125" style="13" customWidth="1"/>
     <col min="9221" max="9221" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="9222" max="9222" width="8" style="13" customWidth="1"/>
     <col min="9223" max="9223" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="10.33203125" style="13" customWidth="1"/>
-    <col min="9225" max="9225" width="9.5" style="13" customWidth="1"/>
-    <col min="9226" max="9226" width="10.1640625" style="13" customWidth="1"/>
-    <col min="9227" max="9227" width="12.5" style="13" customWidth="1"/>
-    <col min="9228" max="9228" width="6.6640625" style="13" customWidth="1"/>
-    <col min="9229" max="9229" width="6.5" style="13" customWidth="1"/>
-    <col min="9230" max="9230" width="6.33203125" style="13" customWidth="1"/>
-    <col min="9231" max="9231" width="12.5" style="13" customWidth="1"/>
-    <col min="9232" max="9232" width="8.1640625" style="13" customWidth="1"/>
-    <col min="9233" max="9234" width="8.5" style="13" customWidth="1"/>
-    <col min="9235" max="9235" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9236" max="9236" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9237" max="9237" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="10.36328125" style="13" customWidth="1"/>
+    <col min="9225" max="9225" width="9.453125" style="13" customWidth="1"/>
+    <col min="9226" max="9226" width="10.1796875" style="13" customWidth="1"/>
+    <col min="9227" max="9227" width="12.453125" style="13" customWidth="1"/>
+    <col min="9228" max="9228" width="6.6328125" style="13" customWidth="1"/>
+    <col min="9229" max="9229" width="6.453125" style="13" customWidth="1"/>
+    <col min="9230" max="9230" width="6.36328125" style="13" customWidth="1"/>
+    <col min="9231" max="9231" width="12.453125" style="13" customWidth="1"/>
+    <col min="9232" max="9232" width="8.1796875" style="13" customWidth="1"/>
+    <col min="9233" max="9234" width="8.453125" style="13" customWidth="1"/>
+    <col min="9235" max="9235" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9236" max="9236" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9237" max="9237" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="9238" max="9238" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="9239" max="9239" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9239" max="9239" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="9240" max="9240" width="18" style="13" customWidth="1"/>
-    <col min="9241" max="9241" width="7.5" style="13" customWidth="1"/>
-    <col min="9242" max="9242" width="10.5" style="13" customWidth="1"/>
-    <col min="9243" max="9472" width="8.83203125" style="13"/>
-    <col min="9473" max="9473" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9241" width="7.453125" style="13" customWidth="1"/>
+    <col min="9242" max="9242" width="10.453125" style="13" customWidth="1"/>
+    <col min="9243" max="9472" width="8.81640625" style="13"/>
+    <col min="9473" max="9473" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="9475" max="9475" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="9476" max="9476" width="7.6640625" style="13" customWidth="1"/>
+    <col min="9476" max="9476" width="7.6328125" style="13" customWidth="1"/>
     <col min="9477" max="9477" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="9478" max="9478" width="8" style="13" customWidth="1"/>
     <col min="9479" max="9479" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="10.33203125" style="13" customWidth="1"/>
-    <col min="9481" max="9481" width="9.5" style="13" customWidth="1"/>
-    <col min="9482" max="9482" width="10.1640625" style="13" customWidth="1"/>
-    <col min="9483" max="9483" width="12.5" style="13" customWidth="1"/>
-    <col min="9484" max="9484" width="6.6640625" style="13" customWidth="1"/>
-    <col min="9485" max="9485" width="6.5" style="13" customWidth="1"/>
-    <col min="9486" max="9486" width="6.33203125" style="13" customWidth="1"/>
-    <col min="9487" max="9487" width="12.5" style="13" customWidth="1"/>
-    <col min="9488" max="9488" width="8.1640625" style="13" customWidth="1"/>
-    <col min="9489" max="9490" width="8.5" style="13" customWidth="1"/>
-    <col min="9491" max="9491" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9492" max="9492" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9493" max="9493" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="10.36328125" style="13" customWidth="1"/>
+    <col min="9481" max="9481" width="9.453125" style="13" customWidth="1"/>
+    <col min="9482" max="9482" width="10.1796875" style="13" customWidth="1"/>
+    <col min="9483" max="9483" width="12.453125" style="13" customWidth="1"/>
+    <col min="9484" max="9484" width="6.6328125" style="13" customWidth="1"/>
+    <col min="9485" max="9485" width="6.453125" style="13" customWidth="1"/>
+    <col min="9486" max="9486" width="6.36328125" style="13" customWidth="1"/>
+    <col min="9487" max="9487" width="12.453125" style="13" customWidth="1"/>
+    <col min="9488" max="9488" width="8.1796875" style="13" customWidth="1"/>
+    <col min="9489" max="9490" width="8.453125" style="13" customWidth="1"/>
+    <col min="9491" max="9491" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9492" max="9492" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9493" max="9493" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="9494" max="9494" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="9495" max="9495" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9495" max="9495" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="9496" max="9496" width="18" style="13" customWidth="1"/>
-    <col min="9497" max="9497" width="7.5" style="13" customWidth="1"/>
-    <col min="9498" max="9498" width="10.5" style="13" customWidth="1"/>
-    <col min="9499" max="9728" width="8.83203125" style="13"/>
-    <col min="9729" max="9729" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9497" width="7.453125" style="13" customWidth="1"/>
+    <col min="9498" max="9498" width="10.453125" style="13" customWidth="1"/>
+    <col min="9499" max="9728" width="8.81640625" style="13"/>
+    <col min="9729" max="9729" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="9731" max="9731" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="9732" max="9732" width="7.6640625" style="13" customWidth="1"/>
+    <col min="9732" max="9732" width="7.6328125" style="13" customWidth="1"/>
     <col min="9733" max="9733" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="9734" max="9734" width="8" style="13" customWidth="1"/>
     <col min="9735" max="9735" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="10.33203125" style="13" customWidth="1"/>
-    <col min="9737" max="9737" width="9.5" style="13" customWidth="1"/>
-    <col min="9738" max="9738" width="10.1640625" style="13" customWidth="1"/>
-    <col min="9739" max="9739" width="12.5" style="13" customWidth="1"/>
-    <col min="9740" max="9740" width="6.6640625" style="13" customWidth="1"/>
-    <col min="9741" max="9741" width="6.5" style="13" customWidth="1"/>
-    <col min="9742" max="9742" width="6.33203125" style="13" customWidth="1"/>
-    <col min="9743" max="9743" width="12.5" style="13" customWidth="1"/>
-    <col min="9744" max="9744" width="8.1640625" style="13" customWidth="1"/>
-    <col min="9745" max="9746" width="8.5" style="13" customWidth="1"/>
-    <col min="9747" max="9747" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9748" max="9748" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9749" max="9749" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="10.36328125" style="13" customWidth="1"/>
+    <col min="9737" max="9737" width="9.453125" style="13" customWidth="1"/>
+    <col min="9738" max="9738" width="10.1796875" style="13" customWidth="1"/>
+    <col min="9739" max="9739" width="12.453125" style="13" customWidth="1"/>
+    <col min="9740" max="9740" width="6.6328125" style="13" customWidth="1"/>
+    <col min="9741" max="9741" width="6.453125" style="13" customWidth="1"/>
+    <col min="9742" max="9742" width="6.36328125" style="13" customWidth="1"/>
+    <col min="9743" max="9743" width="12.453125" style="13" customWidth="1"/>
+    <col min="9744" max="9744" width="8.1796875" style="13" customWidth="1"/>
+    <col min="9745" max="9746" width="8.453125" style="13" customWidth="1"/>
+    <col min="9747" max="9747" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9748" max="9748" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9749" max="9749" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="9750" max="9750" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="9751" max="9751" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9751" max="9751" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="9752" max="9752" width="18" style="13" customWidth="1"/>
-    <col min="9753" max="9753" width="7.5" style="13" customWidth="1"/>
-    <col min="9754" max="9754" width="10.5" style="13" customWidth="1"/>
-    <col min="9755" max="9984" width="8.83203125" style="13"/>
-    <col min="9985" max="9985" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9753" width="7.453125" style="13" customWidth="1"/>
+    <col min="9754" max="9754" width="10.453125" style="13" customWidth="1"/>
+    <col min="9755" max="9984" width="8.81640625" style="13"/>
+    <col min="9985" max="9985" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="9987" max="9987" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="9988" max="9988" width="7.6640625" style="13" customWidth="1"/>
+    <col min="9988" max="9988" width="7.6328125" style="13" customWidth="1"/>
     <col min="9989" max="9989" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="9990" max="9990" width="8" style="13" customWidth="1"/>
     <col min="9991" max="9991" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="10.33203125" style="13" customWidth="1"/>
-    <col min="9993" max="9993" width="9.5" style="13" customWidth="1"/>
-    <col min="9994" max="9994" width="10.1640625" style="13" customWidth="1"/>
-    <col min="9995" max="9995" width="12.5" style="13" customWidth="1"/>
-    <col min="9996" max="9996" width="6.6640625" style="13" customWidth="1"/>
-    <col min="9997" max="9997" width="6.5" style="13" customWidth="1"/>
-    <col min="9998" max="9998" width="6.33203125" style="13" customWidth="1"/>
-    <col min="9999" max="9999" width="12.5" style="13" customWidth="1"/>
-    <col min="10000" max="10000" width="8.1640625" style="13" customWidth="1"/>
-    <col min="10001" max="10002" width="8.5" style="13" customWidth="1"/>
-    <col min="10003" max="10003" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10004" max="10004" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10005" max="10005" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="10.36328125" style="13" customWidth="1"/>
+    <col min="9993" max="9993" width="9.453125" style="13" customWidth="1"/>
+    <col min="9994" max="9994" width="10.1796875" style="13" customWidth="1"/>
+    <col min="9995" max="9995" width="12.453125" style="13" customWidth="1"/>
+    <col min="9996" max="9996" width="6.6328125" style="13" customWidth="1"/>
+    <col min="9997" max="9997" width="6.453125" style="13" customWidth="1"/>
+    <col min="9998" max="9998" width="6.36328125" style="13" customWidth="1"/>
+    <col min="9999" max="9999" width="12.453125" style="13" customWidth="1"/>
+    <col min="10000" max="10000" width="8.1796875" style="13" customWidth="1"/>
+    <col min="10001" max="10002" width="8.453125" style="13" customWidth="1"/>
+    <col min="10003" max="10003" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10004" max="10004" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10005" max="10005" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="10006" max="10006" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="10007" max="10007" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10007" max="10007" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="10008" max="10008" width="18" style="13" customWidth="1"/>
-    <col min="10009" max="10009" width="7.5" style="13" customWidth="1"/>
-    <col min="10010" max="10010" width="10.5" style="13" customWidth="1"/>
-    <col min="10011" max="10240" width="8.83203125" style="13"/>
-    <col min="10241" max="10241" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10009" width="7.453125" style="13" customWidth="1"/>
+    <col min="10010" max="10010" width="10.453125" style="13" customWidth="1"/>
+    <col min="10011" max="10240" width="8.81640625" style="13"/>
+    <col min="10241" max="10241" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="10243" max="10243" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="10244" max="10244" width="7.6640625" style="13" customWidth="1"/>
+    <col min="10244" max="10244" width="7.6328125" style="13" customWidth="1"/>
     <col min="10245" max="10245" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="10246" max="10246" width="8" style="13" customWidth="1"/>
     <col min="10247" max="10247" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="10.33203125" style="13" customWidth="1"/>
-    <col min="10249" max="10249" width="9.5" style="13" customWidth="1"/>
-    <col min="10250" max="10250" width="10.1640625" style="13" customWidth="1"/>
-    <col min="10251" max="10251" width="12.5" style="13" customWidth="1"/>
-    <col min="10252" max="10252" width="6.6640625" style="13" customWidth="1"/>
-    <col min="10253" max="10253" width="6.5" style="13" customWidth="1"/>
-    <col min="10254" max="10254" width="6.33203125" style="13" customWidth="1"/>
-    <col min="10255" max="10255" width="12.5" style="13" customWidth="1"/>
-    <col min="10256" max="10256" width="8.1640625" style="13" customWidth="1"/>
-    <col min="10257" max="10258" width="8.5" style="13" customWidth="1"/>
-    <col min="10259" max="10259" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10260" max="10260" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10261" max="10261" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="10.36328125" style="13" customWidth="1"/>
+    <col min="10249" max="10249" width="9.453125" style="13" customWidth="1"/>
+    <col min="10250" max="10250" width="10.1796875" style="13" customWidth="1"/>
+    <col min="10251" max="10251" width="12.453125" style="13" customWidth="1"/>
+    <col min="10252" max="10252" width="6.6328125" style="13" customWidth="1"/>
+    <col min="10253" max="10253" width="6.453125" style="13" customWidth="1"/>
+    <col min="10254" max="10254" width="6.36328125" style="13" customWidth="1"/>
+    <col min="10255" max="10255" width="12.453125" style="13" customWidth="1"/>
+    <col min="10256" max="10256" width="8.1796875" style="13" customWidth="1"/>
+    <col min="10257" max="10258" width="8.453125" style="13" customWidth="1"/>
+    <col min="10259" max="10259" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10260" max="10260" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10261" max="10261" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="10262" max="10262" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="10263" max="10263" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10263" max="10263" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="10264" max="10264" width="18" style="13" customWidth="1"/>
-    <col min="10265" max="10265" width="7.5" style="13" customWidth="1"/>
-    <col min="10266" max="10266" width="10.5" style="13" customWidth="1"/>
-    <col min="10267" max="10496" width="8.83203125" style="13"/>
-    <col min="10497" max="10497" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10265" width="7.453125" style="13" customWidth="1"/>
+    <col min="10266" max="10266" width="10.453125" style="13" customWidth="1"/>
+    <col min="10267" max="10496" width="8.81640625" style="13"/>
+    <col min="10497" max="10497" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="10499" max="10499" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="10500" max="10500" width="7.6640625" style="13" customWidth="1"/>
+    <col min="10500" max="10500" width="7.6328125" style="13" customWidth="1"/>
     <col min="10501" max="10501" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="10502" max="10502" width="8" style="13" customWidth="1"/>
     <col min="10503" max="10503" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="10.33203125" style="13" customWidth="1"/>
-    <col min="10505" max="10505" width="9.5" style="13" customWidth="1"/>
-    <col min="10506" max="10506" width="10.1640625" style="13" customWidth="1"/>
-    <col min="10507" max="10507" width="12.5" style="13" customWidth="1"/>
-    <col min="10508" max="10508" width="6.6640625" style="13" customWidth="1"/>
-    <col min="10509" max="10509" width="6.5" style="13" customWidth="1"/>
-    <col min="10510" max="10510" width="6.33203125" style="13" customWidth="1"/>
-    <col min="10511" max="10511" width="12.5" style="13" customWidth="1"/>
-    <col min="10512" max="10512" width="8.1640625" style="13" customWidth="1"/>
-    <col min="10513" max="10514" width="8.5" style="13" customWidth="1"/>
-    <col min="10515" max="10515" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10516" max="10516" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10517" max="10517" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="10.36328125" style="13" customWidth="1"/>
+    <col min="10505" max="10505" width="9.453125" style="13" customWidth="1"/>
+    <col min="10506" max="10506" width="10.1796875" style="13" customWidth="1"/>
+    <col min="10507" max="10507" width="12.453125" style="13" customWidth="1"/>
+    <col min="10508" max="10508" width="6.6328125" style="13" customWidth="1"/>
+    <col min="10509" max="10509" width="6.453125" style="13" customWidth="1"/>
+    <col min="10510" max="10510" width="6.36328125" style="13" customWidth="1"/>
+    <col min="10511" max="10511" width="12.453125" style="13" customWidth="1"/>
+    <col min="10512" max="10512" width="8.1796875" style="13" customWidth="1"/>
+    <col min="10513" max="10514" width="8.453125" style="13" customWidth="1"/>
+    <col min="10515" max="10515" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10516" max="10516" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10517" max="10517" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="10518" max="10518" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="10519" max="10519" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10519" max="10519" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="10520" max="10520" width="18" style="13" customWidth="1"/>
-    <col min="10521" max="10521" width="7.5" style="13" customWidth="1"/>
-    <col min="10522" max="10522" width="10.5" style="13" customWidth="1"/>
-    <col min="10523" max="10752" width="8.83203125" style="13"/>
-    <col min="10753" max="10753" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10521" width="7.453125" style="13" customWidth="1"/>
+    <col min="10522" max="10522" width="10.453125" style="13" customWidth="1"/>
+    <col min="10523" max="10752" width="8.81640625" style="13"/>
+    <col min="10753" max="10753" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="10755" max="10755" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="10756" max="10756" width="7.6640625" style="13" customWidth="1"/>
+    <col min="10756" max="10756" width="7.6328125" style="13" customWidth="1"/>
     <col min="10757" max="10757" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="10758" max="10758" width="8" style="13" customWidth="1"/>
     <col min="10759" max="10759" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="10.33203125" style="13" customWidth="1"/>
-    <col min="10761" max="10761" width="9.5" style="13" customWidth="1"/>
-    <col min="10762" max="10762" width="10.1640625" style="13" customWidth="1"/>
-    <col min="10763" max="10763" width="12.5" style="13" customWidth="1"/>
-    <col min="10764" max="10764" width="6.6640625" style="13" customWidth="1"/>
-    <col min="10765" max="10765" width="6.5" style="13" customWidth="1"/>
-    <col min="10766" max="10766" width="6.33203125" style="13" customWidth="1"/>
-    <col min="10767" max="10767" width="12.5" style="13" customWidth="1"/>
-    <col min="10768" max="10768" width="8.1640625" style="13" customWidth="1"/>
-    <col min="10769" max="10770" width="8.5" style="13" customWidth="1"/>
-    <col min="10771" max="10771" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10772" max="10772" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10773" max="10773" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="10.36328125" style="13" customWidth="1"/>
+    <col min="10761" max="10761" width="9.453125" style="13" customWidth="1"/>
+    <col min="10762" max="10762" width="10.1796875" style="13" customWidth="1"/>
+    <col min="10763" max="10763" width="12.453125" style="13" customWidth="1"/>
+    <col min="10764" max="10764" width="6.6328125" style="13" customWidth="1"/>
+    <col min="10765" max="10765" width="6.453125" style="13" customWidth="1"/>
+    <col min="10766" max="10766" width="6.36328125" style="13" customWidth="1"/>
+    <col min="10767" max="10767" width="12.453125" style="13" customWidth="1"/>
+    <col min="10768" max="10768" width="8.1796875" style="13" customWidth="1"/>
+    <col min="10769" max="10770" width="8.453125" style="13" customWidth="1"/>
+    <col min="10771" max="10771" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10772" max="10772" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10773" max="10773" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="10774" max="10774" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="10775" max="10775" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10775" max="10775" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="10776" max="10776" width="18" style="13" customWidth="1"/>
-    <col min="10777" max="10777" width="7.5" style="13" customWidth="1"/>
-    <col min="10778" max="10778" width="10.5" style="13" customWidth="1"/>
-    <col min="10779" max="11008" width="8.83203125" style="13"/>
-    <col min="11009" max="11009" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10777" max="10777" width="7.453125" style="13" customWidth="1"/>
+    <col min="10778" max="10778" width="10.453125" style="13" customWidth="1"/>
+    <col min="10779" max="11008" width="8.81640625" style="13"/>
+    <col min="11009" max="11009" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11011" max="11011" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="11012" max="11012" width="7.6640625" style="13" customWidth="1"/>
+    <col min="11012" max="11012" width="7.6328125" style="13" customWidth="1"/>
     <col min="11013" max="11013" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="11014" max="11014" width="8" style="13" customWidth="1"/>
     <col min="11015" max="11015" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="10.33203125" style="13" customWidth="1"/>
-    <col min="11017" max="11017" width="9.5" style="13" customWidth="1"/>
-    <col min="11018" max="11018" width="10.1640625" style="13" customWidth="1"/>
-    <col min="11019" max="11019" width="12.5" style="13" customWidth="1"/>
-    <col min="11020" max="11020" width="6.6640625" style="13" customWidth="1"/>
-    <col min="11021" max="11021" width="6.5" style="13" customWidth="1"/>
-    <col min="11022" max="11022" width="6.33203125" style="13" customWidth="1"/>
-    <col min="11023" max="11023" width="12.5" style="13" customWidth="1"/>
-    <col min="11024" max="11024" width="8.1640625" style="13" customWidth="1"/>
-    <col min="11025" max="11026" width="8.5" style="13" customWidth="1"/>
-    <col min="11027" max="11027" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11028" max="11028" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11029" max="11029" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="10.36328125" style="13" customWidth="1"/>
+    <col min="11017" max="11017" width="9.453125" style="13" customWidth="1"/>
+    <col min="11018" max="11018" width="10.1796875" style="13" customWidth="1"/>
+    <col min="11019" max="11019" width="12.453125" style="13" customWidth="1"/>
+    <col min="11020" max="11020" width="6.6328125" style="13" customWidth="1"/>
+    <col min="11021" max="11021" width="6.453125" style="13" customWidth="1"/>
+    <col min="11022" max="11022" width="6.36328125" style="13" customWidth="1"/>
+    <col min="11023" max="11023" width="12.453125" style="13" customWidth="1"/>
+    <col min="11024" max="11024" width="8.1796875" style="13" customWidth="1"/>
+    <col min="11025" max="11026" width="8.453125" style="13" customWidth="1"/>
+    <col min="11027" max="11027" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11028" max="11028" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11029" max="11029" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="11030" max="11030" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="11031" max="11031" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11031" max="11031" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11032" max="11032" width="18" style="13" customWidth="1"/>
-    <col min="11033" max="11033" width="7.5" style="13" customWidth="1"/>
-    <col min="11034" max="11034" width="10.5" style="13" customWidth="1"/>
-    <col min="11035" max="11264" width="8.83203125" style="13"/>
-    <col min="11265" max="11265" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11033" width="7.453125" style="13" customWidth="1"/>
+    <col min="11034" max="11034" width="10.453125" style="13" customWidth="1"/>
+    <col min="11035" max="11264" width="8.81640625" style="13"/>
+    <col min="11265" max="11265" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11267" max="11267" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="11268" max="11268" width="7.6640625" style="13" customWidth="1"/>
+    <col min="11268" max="11268" width="7.6328125" style="13" customWidth="1"/>
     <col min="11269" max="11269" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="11270" max="11270" width="8" style="13" customWidth="1"/>
     <col min="11271" max="11271" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="10.33203125" style="13" customWidth="1"/>
-    <col min="11273" max="11273" width="9.5" style="13" customWidth="1"/>
-    <col min="11274" max="11274" width="10.1640625" style="13" customWidth="1"/>
-    <col min="11275" max="11275" width="12.5" style="13" customWidth="1"/>
-    <col min="11276" max="11276" width="6.6640625" style="13" customWidth="1"/>
-    <col min="11277" max="11277" width="6.5" style="13" customWidth="1"/>
-    <col min="11278" max="11278" width="6.33203125" style="13" customWidth="1"/>
-    <col min="11279" max="11279" width="12.5" style="13" customWidth="1"/>
-    <col min="11280" max="11280" width="8.1640625" style="13" customWidth="1"/>
-    <col min="11281" max="11282" width="8.5" style="13" customWidth="1"/>
-    <col min="11283" max="11283" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11284" max="11284" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11285" max="11285" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="10.36328125" style="13" customWidth="1"/>
+    <col min="11273" max="11273" width="9.453125" style="13" customWidth="1"/>
+    <col min="11274" max="11274" width="10.1796875" style="13" customWidth="1"/>
+    <col min="11275" max="11275" width="12.453125" style="13" customWidth="1"/>
+    <col min="11276" max="11276" width="6.6328125" style="13" customWidth="1"/>
+    <col min="11277" max="11277" width="6.453125" style="13" customWidth="1"/>
+    <col min="11278" max="11278" width="6.36328125" style="13" customWidth="1"/>
+    <col min="11279" max="11279" width="12.453125" style="13" customWidth="1"/>
+    <col min="11280" max="11280" width="8.1796875" style="13" customWidth="1"/>
+    <col min="11281" max="11282" width="8.453125" style="13" customWidth="1"/>
+    <col min="11283" max="11283" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11284" max="11284" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11285" max="11285" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="11286" max="11286" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="11287" max="11287" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11287" max="11287" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11288" max="11288" width="18" style="13" customWidth="1"/>
-    <col min="11289" max="11289" width="7.5" style="13" customWidth="1"/>
-    <col min="11290" max="11290" width="10.5" style="13" customWidth="1"/>
-    <col min="11291" max="11520" width="8.83203125" style="13"/>
-    <col min="11521" max="11521" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11289" width="7.453125" style="13" customWidth="1"/>
+    <col min="11290" max="11290" width="10.453125" style="13" customWidth="1"/>
+    <col min="11291" max="11520" width="8.81640625" style="13"/>
+    <col min="11521" max="11521" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11523" max="11523" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="11524" max="11524" width="7.6640625" style="13" customWidth="1"/>
+    <col min="11524" max="11524" width="7.6328125" style="13" customWidth="1"/>
     <col min="11525" max="11525" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="11526" max="11526" width="8" style="13" customWidth="1"/>
     <col min="11527" max="11527" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="10.33203125" style="13" customWidth="1"/>
-    <col min="11529" max="11529" width="9.5" style="13" customWidth="1"/>
-    <col min="11530" max="11530" width="10.1640625" style="13" customWidth="1"/>
-    <col min="11531" max="11531" width="12.5" style="13" customWidth="1"/>
-    <col min="11532" max="11532" width="6.6640625" style="13" customWidth="1"/>
-    <col min="11533" max="11533" width="6.5" style="13" customWidth="1"/>
-    <col min="11534" max="11534" width="6.33203125" style="13" customWidth="1"/>
-    <col min="11535" max="11535" width="12.5" style="13" customWidth="1"/>
-    <col min="11536" max="11536" width="8.1640625" style="13" customWidth="1"/>
-    <col min="11537" max="11538" width="8.5" style="13" customWidth="1"/>
-    <col min="11539" max="11539" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11540" max="11540" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11541" max="11541" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="10.36328125" style="13" customWidth="1"/>
+    <col min="11529" max="11529" width="9.453125" style="13" customWidth="1"/>
+    <col min="11530" max="11530" width="10.1796875" style="13" customWidth="1"/>
+    <col min="11531" max="11531" width="12.453125" style="13" customWidth="1"/>
+    <col min="11532" max="11532" width="6.6328125" style="13" customWidth="1"/>
+    <col min="11533" max="11533" width="6.453125" style="13" customWidth="1"/>
+    <col min="11534" max="11534" width="6.36328125" style="13" customWidth="1"/>
+    <col min="11535" max="11535" width="12.453125" style="13" customWidth="1"/>
+    <col min="11536" max="11536" width="8.1796875" style="13" customWidth="1"/>
+    <col min="11537" max="11538" width="8.453125" style="13" customWidth="1"/>
+    <col min="11539" max="11539" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11540" max="11540" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11541" max="11541" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="11542" max="11542" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="11543" max="11543" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11543" max="11543" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11544" max="11544" width="18" style="13" customWidth="1"/>
-    <col min="11545" max="11545" width="7.5" style="13" customWidth="1"/>
-    <col min="11546" max="11546" width="10.5" style="13" customWidth="1"/>
-    <col min="11547" max="11776" width="8.83203125" style="13"/>
-    <col min="11777" max="11777" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11545" width="7.453125" style="13" customWidth="1"/>
+    <col min="11546" max="11546" width="10.453125" style="13" customWidth="1"/>
+    <col min="11547" max="11776" width="8.81640625" style="13"/>
+    <col min="11777" max="11777" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11779" max="11779" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="11780" max="11780" width="7.6640625" style="13" customWidth="1"/>
+    <col min="11780" max="11780" width="7.6328125" style="13" customWidth="1"/>
     <col min="11781" max="11781" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="11782" max="11782" width="8" style="13" customWidth="1"/>
     <col min="11783" max="11783" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="10.33203125" style="13" customWidth="1"/>
-    <col min="11785" max="11785" width="9.5" style="13" customWidth="1"/>
-    <col min="11786" max="11786" width="10.1640625" style="13" customWidth="1"/>
-    <col min="11787" max="11787" width="12.5" style="13" customWidth="1"/>
-    <col min="11788" max="11788" width="6.6640625" style="13" customWidth="1"/>
-    <col min="11789" max="11789" width="6.5" style="13" customWidth="1"/>
-    <col min="11790" max="11790" width="6.33203125" style="13" customWidth="1"/>
-    <col min="11791" max="11791" width="12.5" style="13" customWidth="1"/>
-    <col min="11792" max="11792" width="8.1640625" style="13" customWidth="1"/>
-    <col min="11793" max="11794" width="8.5" style="13" customWidth="1"/>
-    <col min="11795" max="11795" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11796" max="11796" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11797" max="11797" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="10.36328125" style="13" customWidth="1"/>
+    <col min="11785" max="11785" width="9.453125" style="13" customWidth="1"/>
+    <col min="11786" max="11786" width="10.1796875" style="13" customWidth="1"/>
+    <col min="11787" max="11787" width="12.453125" style="13" customWidth="1"/>
+    <col min="11788" max="11788" width="6.6328125" style="13" customWidth="1"/>
+    <col min="11789" max="11789" width="6.453125" style="13" customWidth="1"/>
+    <col min="11790" max="11790" width="6.36328125" style="13" customWidth="1"/>
+    <col min="11791" max="11791" width="12.453125" style="13" customWidth="1"/>
+    <col min="11792" max="11792" width="8.1796875" style="13" customWidth="1"/>
+    <col min="11793" max="11794" width="8.453125" style="13" customWidth="1"/>
+    <col min="11795" max="11795" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11796" max="11796" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11797" max="11797" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="11798" max="11798" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="11799" max="11799" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11799" max="11799" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="11800" max="11800" width="18" style="13" customWidth="1"/>
-    <col min="11801" max="11801" width="7.5" style="13" customWidth="1"/>
-    <col min="11802" max="11802" width="10.5" style="13" customWidth="1"/>
-    <col min="11803" max="12032" width="8.83203125" style="13"/>
-    <col min="12033" max="12033" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="11801" max="11801" width="7.453125" style="13" customWidth="1"/>
+    <col min="11802" max="11802" width="10.453125" style="13" customWidth="1"/>
+    <col min="11803" max="12032" width="8.81640625" style="13"/>
+    <col min="12033" max="12033" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12035" max="12035" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="12036" max="12036" width="7.6640625" style="13" customWidth="1"/>
+    <col min="12036" max="12036" width="7.6328125" style="13" customWidth="1"/>
     <col min="12037" max="12037" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="12038" max="12038" width="8" style="13" customWidth="1"/>
     <col min="12039" max="12039" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="10.33203125" style="13" customWidth="1"/>
-    <col min="12041" max="12041" width="9.5" style="13" customWidth="1"/>
-    <col min="12042" max="12042" width="10.1640625" style="13" customWidth="1"/>
-    <col min="12043" max="12043" width="12.5" style="13" customWidth="1"/>
-    <col min="12044" max="12044" width="6.6640625" style="13" customWidth="1"/>
-    <col min="12045" max="12045" width="6.5" style="13" customWidth="1"/>
-    <col min="12046" max="12046" width="6.33203125" style="13" customWidth="1"/>
-    <col min="12047" max="12047" width="12.5" style="13" customWidth="1"/>
-    <col min="12048" max="12048" width="8.1640625" style="13" customWidth="1"/>
-    <col min="12049" max="12050" width="8.5" style="13" customWidth="1"/>
-    <col min="12051" max="12051" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12052" max="12052" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12053" max="12053" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="10.36328125" style="13" customWidth="1"/>
+    <col min="12041" max="12041" width="9.453125" style="13" customWidth="1"/>
+    <col min="12042" max="12042" width="10.1796875" style="13" customWidth="1"/>
+    <col min="12043" max="12043" width="12.453125" style="13" customWidth="1"/>
+    <col min="12044" max="12044" width="6.6328125" style="13" customWidth="1"/>
+    <col min="12045" max="12045" width="6.453125" style="13" customWidth="1"/>
+    <col min="12046" max="12046" width="6.36328125" style="13" customWidth="1"/>
+    <col min="12047" max="12047" width="12.453125" style="13" customWidth="1"/>
+    <col min="12048" max="12048" width="8.1796875" style="13" customWidth="1"/>
+    <col min="12049" max="12050" width="8.453125" style="13" customWidth="1"/>
+    <col min="12051" max="12051" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12052" max="12052" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12053" max="12053" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="12054" max="12054" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="12055" max="12055" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12055" max="12055" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12056" max="12056" width="18" style="13" customWidth="1"/>
-    <col min="12057" max="12057" width="7.5" style="13" customWidth="1"/>
-    <col min="12058" max="12058" width="10.5" style="13" customWidth="1"/>
-    <col min="12059" max="12288" width="8.83203125" style="13"/>
-    <col min="12289" max="12289" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12057" width="7.453125" style="13" customWidth="1"/>
+    <col min="12058" max="12058" width="10.453125" style="13" customWidth="1"/>
+    <col min="12059" max="12288" width="8.81640625" style="13"/>
+    <col min="12289" max="12289" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12291" max="12291" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="12292" max="12292" width="7.6640625" style="13" customWidth="1"/>
+    <col min="12292" max="12292" width="7.6328125" style="13" customWidth="1"/>
     <col min="12293" max="12293" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="12294" max="12294" width="8" style="13" customWidth="1"/>
     <col min="12295" max="12295" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="10.33203125" style="13" customWidth="1"/>
-    <col min="12297" max="12297" width="9.5" style="13" customWidth="1"/>
-    <col min="12298" max="12298" width="10.1640625" style="13" customWidth="1"/>
-    <col min="12299" max="12299" width="12.5" style="13" customWidth="1"/>
-    <col min="12300" max="12300" width="6.6640625" style="13" customWidth="1"/>
-    <col min="12301" max="12301" width="6.5" style="13" customWidth="1"/>
-    <col min="12302" max="12302" width="6.33203125" style="13" customWidth="1"/>
-    <col min="12303" max="12303" width="12.5" style="13" customWidth="1"/>
-    <col min="12304" max="12304" width="8.1640625" style="13" customWidth="1"/>
-    <col min="12305" max="12306" width="8.5" style="13" customWidth="1"/>
-    <col min="12307" max="12307" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12308" max="12308" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12309" max="12309" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="10.36328125" style="13" customWidth="1"/>
+    <col min="12297" max="12297" width="9.453125" style="13" customWidth="1"/>
+    <col min="12298" max="12298" width="10.1796875" style="13" customWidth="1"/>
+    <col min="12299" max="12299" width="12.453125" style="13" customWidth="1"/>
+    <col min="12300" max="12300" width="6.6328125" style="13" customWidth="1"/>
+    <col min="12301" max="12301" width="6.453125" style="13" customWidth="1"/>
+    <col min="12302" max="12302" width="6.36328125" style="13" customWidth="1"/>
+    <col min="12303" max="12303" width="12.453125" style="13" customWidth="1"/>
+    <col min="12304" max="12304" width="8.1796875" style="13" customWidth="1"/>
+    <col min="12305" max="12306" width="8.453125" style="13" customWidth="1"/>
+    <col min="12307" max="12307" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12308" max="12308" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12309" max="12309" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="12310" max="12310" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="12311" max="12311" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12311" max="12311" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12312" max="12312" width="18" style="13" customWidth="1"/>
-    <col min="12313" max="12313" width="7.5" style="13" customWidth="1"/>
-    <col min="12314" max="12314" width="10.5" style="13" customWidth="1"/>
-    <col min="12315" max="12544" width="8.83203125" style="13"/>
-    <col min="12545" max="12545" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12313" width="7.453125" style="13" customWidth="1"/>
+    <col min="12314" max="12314" width="10.453125" style="13" customWidth="1"/>
+    <col min="12315" max="12544" width="8.81640625" style="13"/>
+    <col min="12545" max="12545" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12547" max="12547" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="12548" max="12548" width="7.6640625" style="13" customWidth="1"/>
+    <col min="12548" max="12548" width="7.6328125" style="13" customWidth="1"/>
     <col min="12549" max="12549" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="12550" max="12550" width="8" style="13" customWidth="1"/>
     <col min="12551" max="12551" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="10.33203125" style="13" customWidth="1"/>
-    <col min="12553" max="12553" width="9.5" style="13" customWidth="1"/>
-    <col min="12554" max="12554" width="10.1640625" style="13" customWidth="1"/>
-    <col min="12555" max="12555" width="12.5" style="13" customWidth="1"/>
-    <col min="12556" max="12556" width="6.6640625" style="13" customWidth="1"/>
-    <col min="12557" max="12557" width="6.5" style="13" customWidth="1"/>
-    <col min="12558" max="12558" width="6.33203125" style="13" customWidth="1"/>
-    <col min="12559" max="12559" width="12.5" style="13" customWidth="1"/>
-    <col min="12560" max="12560" width="8.1640625" style="13" customWidth="1"/>
-    <col min="12561" max="12562" width="8.5" style="13" customWidth="1"/>
-    <col min="12563" max="12563" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12564" max="12564" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12565" max="12565" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="10.36328125" style="13" customWidth="1"/>
+    <col min="12553" max="12553" width="9.453125" style="13" customWidth="1"/>
+    <col min="12554" max="12554" width="10.1796875" style="13" customWidth="1"/>
+    <col min="12555" max="12555" width="12.453125" style="13" customWidth="1"/>
+    <col min="12556" max="12556" width="6.6328125" style="13" customWidth="1"/>
+    <col min="12557" max="12557" width="6.453125" style="13" customWidth="1"/>
+    <col min="12558" max="12558" width="6.36328125" style="13" customWidth="1"/>
+    <col min="12559" max="12559" width="12.453125" style="13" customWidth="1"/>
+    <col min="12560" max="12560" width="8.1796875" style="13" customWidth="1"/>
+    <col min="12561" max="12562" width="8.453125" style="13" customWidth="1"/>
+    <col min="12563" max="12563" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12564" max="12564" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12565" max="12565" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="12566" max="12566" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="12567" max="12567" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12567" max="12567" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12568" max="12568" width="18" style="13" customWidth="1"/>
-    <col min="12569" max="12569" width="7.5" style="13" customWidth="1"/>
-    <col min="12570" max="12570" width="10.5" style="13" customWidth="1"/>
-    <col min="12571" max="12800" width="8.83203125" style="13"/>
-    <col min="12801" max="12801" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12569" width="7.453125" style="13" customWidth="1"/>
+    <col min="12570" max="12570" width="10.453125" style="13" customWidth="1"/>
+    <col min="12571" max="12800" width="8.81640625" style="13"/>
+    <col min="12801" max="12801" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12803" max="12803" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="12804" max="12804" width="7.6640625" style="13" customWidth="1"/>
+    <col min="12804" max="12804" width="7.6328125" style="13" customWidth="1"/>
     <col min="12805" max="12805" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="12806" max="12806" width="8" style="13" customWidth="1"/>
     <col min="12807" max="12807" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="10.33203125" style="13" customWidth="1"/>
-    <col min="12809" max="12809" width="9.5" style="13" customWidth="1"/>
-    <col min="12810" max="12810" width="10.1640625" style="13" customWidth="1"/>
-    <col min="12811" max="12811" width="12.5" style="13" customWidth="1"/>
-    <col min="12812" max="12812" width="6.6640625" style="13" customWidth="1"/>
-    <col min="12813" max="12813" width="6.5" style="13" customWidth="1"/>
-    <col min="12814" max="12814" width="6.33203125" style="13" customWidth="1"/>
-    <col min="12815" max="12815" width="12.5" style="13" customWidth="1"/>
-    <col min="12816" max="12816" width="8.1640625" style="13" customWidth="1"/>
-    <col min="12817" max="12818" width="8.5" style="13" customWidth="1"/>
-    <col min="12819" max="12819" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12820" max="12820" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12821" max="12821" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="10.36328125" style="13" customWidth="1"/>
+    <col min="12809" max="12809" width="9.453125" style="13" customWidth="1"/>
+    <col min="12810" max="12810" width="10.1796875" style="13" customWidth="1"/>
+    <col min="12811" max="12811" width="12.453125" style="13" customWidth="1"/>
+    <col min="12812" max="12812" width="6.6328125" style="13" customWidth="1"/>
+    <col min="12813" max="12813" width="6.453125" style="13" customWidth="1"/>
+    <col min="12814" max="12814" width="6.36328125" style="13" customWidth="1"/>
+    <col min="12815" max="12815" width="12.453125" style="13" customWidth="1"/>
+    <col min="12816" max="12816" width="8.1796875" style="13" customWidth="1"/>
+    <col min="12817" max="12818" width="8.453125" style="13" customWidth="1"/>
+    <col min="12819" max="12819" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12820" max="12820" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="12821" max="12821" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="12822" max="12822" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="12823" max="12823" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12823" max="12823" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="12824" max="12824" width="18" style="13" customWidth="1"/>
-    <col min="12825" max="12825" width="7.5" style="13" customWidth="1"/>
-    <col min="12826" max="12826" width="10.5" style="13" customWidth="1"/>
-    <col min="12827" max="13056" width="8.83203125" style="13"/>
-    <col min="13057" max="13057" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="12825" max="12825" width="7.453125" style="13" customWidth="1"/>
+    <col min="12826" max="12826" width="10.453125" style="13" customWidth="1"/>
+    <col min="12827" max="13056" width="8.81640625" style="13"/>
+    <col min="13057" max="13057" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13059" max="13059" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="13060" max="13060" width="7.6640625" style="13" customWidth="1"/>
+    <col min="13060" max="13060" width="7.6328125" style="13" customWidth="1"/>
     <col min="13061" max="13061" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="13062" max="13062" width="8" style="13" customWidth="1"/>
     <col min="13063" max="13063" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="10.33203125" style="13" customWidth="1"/>
-    <col min="13065" max="13065" width="9.5" style="13" customWidth="1"/>
-    <col min="13066" max="13066" width="10.1640625" style="13" customWidth="1"/>
-    <col min="13067" max="13067" width="12.5" style="13" customWidth="1"/>
-    <col min="13068" max="13068" width="6.6640625" style="13" customWidth="1"/>
-    <col min="13069" max="13069" width="6.5" style="13" customWidth="1"/>
-    <col min="13070" max="13070" width="6.33203125" style="13" customWidth="1"/>
-    <col min="13071" max="13071" width="12.5" style="13" customWidth="1"/>
-    <col min="13072" max="13072" width="8.1640625" style="13" customWidth="1"/>
-    <col min="13073" max="13074" width="8.5" style="13" customWidth="1"/>
-    <col min="13075" max="13075" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13076" max="13076" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13077" max="13077" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="10.36328125" style="13" customWidth="1"/>
+    <col min="13065" max="13065" width="9.453125" style="13" customWidth="1"/>
+    <col min="13066" max="13066" width="10.1796875" style="13" customWidth="1"/>
+    <col min="13067" max="13067" width="12.453125" style="13" customWidth="1"/>
+    <col min="13068" max="13068" width="6.6328125" style="13" customWidth="1"/>
+    <col min="13069" max="13069" width="6.453125" style="13" customWidth="1"/>
+    <col min="13070" max="13070" width="6.36328125" style="13" customWidth="1"/>
+    <col min="13071" max="13071" width="12.453125" style="13" customWidth="1"/>
+    <col min="13072" max="13072" width="8.1796875" style="13" customWidth="1"/>
+    <col min="13073" max="13074" width="8.453125" style="13" customWidth="1"/>
+    <col min="13075" max="13075" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13076" max="13076" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="13077" max="13077" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="13078" max="13078" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="13079" max="13079" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13079" max="13079" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13080" max="13080" width="18" style="13" customWidth="1"/>
-    <col min="13081" max="13081" width="7.5" style="13" customWidth="1"/>
-    <col min="13082" max="13082" width="10.5" style="13" customWidth="1"/>
-    <col min="13083" max="13312" width="8.83203125" style="13"/>
-    <col min="13313" max="13313" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13081" width="7.453125" style="13" customWidth="1"/>
+    <col min="13082" max="13082" width="10.453125" style="13" customWidth="1"/>
+    <col min="13083" max="13312" width="8.81640625" style="13"/>
+    <col min="13313" max="13313" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13315" max="13315" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="13316" max="13316" width="7.6640625" style="13" customWidth="1"/>
+    <col min="13316" max="13316" width="7.6328125" style="13" customWidth="1"/>
     <col min="13317" max="13317" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="13318" max="13318" width="8" style="13" customWidth="1"/>
     <col min="13319" max="13319" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="10.33203125" style="13" customWidth="1"/>
-    <col min="13321" max="13321" width="9.5" style="13" customWidth="1"/>
-    <col min="13322" max="13322" width="10.1640625" style="13" customWidth="1"/>
-    <col min="13323" max="13323" width="12.5" style="13" customWidth="1"/>
-    <col min="13324" max="13324" width="6.6640625" style="13" customWidth="1"/>
-    <col min="13325" max="13325" width="6.5" style="13" customWidth="1"/>
-    <col min="13326" max="13326" width="6.33203125" style="13" customWidth="1"/>
-    <col min="13327" max="13327" width="12.5" style="13" customWidth="1"/>
-    <col min="13328" max="13328" width="8.1640625" style="13" customWidth="1"/>
-    <col min="13329" max="13330" width="8.5" style="13" customWidth="1"/>
-    <col min="13331" max="13331" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13332" max="13332" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13333" max="13333" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="10.36328125" style="13" customWidth="1"/>
+    <col min="13321" max="13321" width="9.453125" style="13" customWidth="1"/>
+    <col min="13322" max="13322" width="10.1796875" style="13" customWidth="1"/>
+    <col min="13323" max="13323" width="12.453125" style="13" customWidth="1"/>
+    <col min="13324" max="13324" width="6.6328125" style="13" customWidth="1"/>
+    <col min="13325" max="13325" width="6.453125" style="13" customWidth="1"/>
+    <col min="13326" max="13326" width="6.36328125" style="13" customWidth="1"/>
+    <col min="13327" max="13327" width="12.453125" style="13" customWidth="1"/>
+    <col min="13328" max="13328" width="8.1796875" style="13" customWidth="1"/>
+    <col min="13329" max="13330" width="8.453125" style="13" customWidth="1"/>
+    <col min="13331" max="13331" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13332" max="13332" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="13333" max="13333" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="13334" max="13334" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="13335" max="13335" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13335" max="13335" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13336" max="13336" width="18" style="13" customWidth="1"/>
-    <col min="13337" max="13337" width="7.5" style="13" customWidth="1"/>
-    <col min="13338" max="13338" width="10.5" style="13" customWidth="1"/>
-    <col min="13339" max="13568" width="8.83203125" style="13"/>
-    <col min="13569" max="13569" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13337" width="7.453125" style="13" customWidth="1"/>
+    <col min="13338" max="13338" width="10.453125" style="13" customWidth="1"/>
+    <col min="13339" max="13568" width="8.81640625" style="13"/>
+    <col min="13569" max="13569" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13571" max="13571" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="13572" max="13572" width="7.6640625" style="13" customWidth="1"/>
+    <col min="13572" max="13572" width="7.6328125" style="13" customWidth="1"/>
     <col min="13573" max="13573" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="13574" max="13574" width="8" style="13" customWidth="1"/>
     <col min="13575" max="13575" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="10.33203125" style="13" customWidth="1"/>
-    <col min="13577" max="13577" width="9.5" style="13" customWidth="1"/>
-    <col min="13578" max="13578" width="10.1640625" style="13" customWidth="1"/>
-    <col min="13579" max="13579" width="12.5" style="13" customWidth="1"/>
-    <col min="13580" max="13580" width="6.6640625" style="13" customWidth="1"/>
-    <col min="13581" max="13581" width="6.5" style="13" customWidth="1"/>
-    <col min="13582" max="13582" width="6.33203125" style="13" customWidth="1"/>
-    <col min="13583" max="13583" width="12.5" style="13" customWidth="1"/>
-    <col min="13584" max="13584" width="8.1640625" style="13" customWidth="1"/>
-    <col min="13585" max="13586" width="8.5" style="13" customWidth="1"/>
-    <col min="13587" max="13587" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13588" max="13588" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13589" max="13589" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="10.36328125" style="13" customWidth="1"/>
+    <col min="13577" max="13577" width="9.453125" style="13" customWidth="1"/>
+    <col min="13578" max="13578" width="10.1796875" style="13" customWidth="1"/>
+    <col min="13579" max="13579" width="12.453125" style="13" customWidth="1"/>
+    <col min="13580" max="13580" width="6.6328125" style="13" customWidth="1"/>
+    <col min="13581" max="13581" width="6.453125" style="13" customWidth="1"/>
+    <col min="13582" max="13582" width="6.36328125" style="13" customWidth="1"/>
+    <col min="13583" max="13583" width="12.453125" style="13" customWidth="1"/>
+    <col min="13584" max="13584" width="8.1796875" style="13" customWidth="1"/>
+    <col min="13585" max="13586" width="8.453125" style="13" customWidth="1"/>
+    <col min="13587" max="13587" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13588" max="13588" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="13589" max="13589" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="13590" max="13590" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="13591" max="13591" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13591" max="13591" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13592" max="13592" width="18" style="13" customWidth="1"/>
-    <col min="13593" max="13593" width="7.5" style="13" customWidth="1"/>
-    <col min="13594" max="13594" width="10.5" style="13" customWidth="1"/>
-    <col min="13595" max="13824" width="8.83203125" style="13"/>
-    <col min="13825" max="13825" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13593" width="7.453125" style="13" customWidth="1"/>
+    <col min="13594" max="13594" width="10.453125" style="13" customWidth="1"/>
+    <col min="13595" max="13824" width="8.81640625" style="13"/>
+    <col min="13825" max="13825" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13827" max="13827" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="13828" max="13828" width="7.6640625" style="13" customWidth="1"/>
+    <col min="13828" max="13828" width="7.6328125" style="13" customWidth="1"/>
     <col min="13829" max="13829" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="13830" max="13830" width="8" style="13" customWidth="1"/>
     <col min="13831" max="13831" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="10.33203125" style="13" customWidth="1"/>
-    <col min="13833" max="13833" width="9.5" style="13" customWidth="1"/>
-    <col min="13834" max="13834" width="10.1640625" style="13" customWidth="1"/>
-    <col min="13835" max="13835" width="12.5" style="13" customWidth="1"/>
-    <col min="13836" max="13836" width="6.6640625" style="13" customWidth="1"/>
-    <col min="13837" max="13837" width="6.5" style="13" customWidth="1"/>
-    <col min="13838" max="13838" width="6.33203125" style="13" customWidth="1"/>
-    <col min="13839" max="13839" width="12.5" style="13" customWidth="1"/>
-    <col min="13840" max="13840" width="8.1640625" style="13" customWidth="1"/>
-    <col min="13841" max="13842" width="8.5" style="13" customWidth="1"/>
-    <col min="13843" max="13843" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13844" max="13844" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13845" max="13845" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="10.36328125" style="13" customWidth="1"/>
+    <col min="13833" max="13833" width="9.453125" style="13" customWidth="1"/>
+    <col min="13834" max="13834" width="10.1796875" style="13" customWidth="1"/>
+    <col min="13835" max="13835" width="12.453125" style="13" customWidth="1"/>
+    <col min="13836" max="13836" width="6.6328125" style="13" customWidth="1"/>
+    <col min="13837" max="13837" width="6.453125" style="13" customWidth="1"/>
+    <col min="13838" max="13838" width="6.36328125" style="13" customWidth="1"/>
+    <col min="13839" max="13839" width="12.453125" style="13" customWidth="1"/>
+    <col min="13840" max="13840" width="8.1796875" style="13" customWidth="1"/>
+    <col min="13841" max="13842" width="8.453125" style="13" customWidth="1"/>
+    <col min="13843" max="13843" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="13844" max="13844" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="13845" max="13845" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="13846" max="13846" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="13847" max="13847" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13847" max="13847" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="13848" max="13848" width="18" style="13" customWidth="1"/>
-    <col min="13849" max="13849" width="7.5" style="13" customWidth="1"/>
-    <col min="13850" max="13850" width="10.5" style="13" customWidth="1"/>
-    <col min="13851" max="14080" width="8.83203125" style="13"/>
-    <col min="14081" max="14081" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="13849" max="13849" width="7.453125" style="13" customWidth="1"/>
+    <col min="13850" max="13850" width="10.453125" style="13" customWidth="1"/>
+    <col min="13851" max="14080" width="8.81640625" style="13"/>
+    <col min="14081" max="14081" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14083" max="14083" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="14084" max="14084" width="7.6640625" style="13" customWidth="1"/>
+    <col min="14084" max="14084" width="7.6328125" style="13" customWidth="1"/>
     <col min="14085" max="14085" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="14086" max="14086" width="8" style="13" customWidth="1"/>
     <col min="14087" max="14087" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="10.33203125" style="13" customWidth="1"/>
-    <col min="14089" max="14089" width="9.5" style="13" customWidth="1"/>
-    <col min="14090" max="14090" width="10.1640625" style="13" customWidth="1"/>
-    <col min="14091" max="14091" width="12.5" style="13" customWidth="1"/>
-    <col min="14092" max="14092" width="6.6640625" style="13" customWidth="1"/>
-    <col min="14093" max="14093" width="6.5" style="13" customWidth="1"/>
-    <col min="14094" max="14094" width="6.33203125" style="13" customWidth="1"/>
-    <col min="14095" max="14095" width="12.5" style="13" customWidth="1"/>
-    <col min="14096" max="14096" width="8.1640625" style="13" customWidth="1"/>
-    <col min="14097" max="14098" width="8.5" style="13" customWidth="1"/>
-    <col min="14099" max="14099" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14100" max="14100" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14101" max="14101" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="10.36328125" style="13" customWidth="1"/>
+    <col min="14089" max="14089" width="9.453125" style="13" customWidth="1"/>
+    <col min="14090" max="14090" width="10.1796875" style="13" customWidth="1"/>
+    <col min="14091" max="14091" width="12.453125" style="13" customWidth="1"/>
+    <col min="14092" max="14092" width="6.6328125" style="13" customWidth="1"/>
+    <col min="14093" max="14093" width="6.453125" style="13" customWidth="1"/>
+    <col min="14094" max="14094" width="6.36328125" style="13" customWidth="1"/>
+    <col min="14095" max="14095" width="12.453125" style="13" customWidth="1"/>
+    <col min="14096" max="14096" width="8.1796875" style="13" customWidth="1"/>
+    <col min="14097" max="14098" width="8.453125" style="13" customWidth="1"/>
+    <col min="14099" max="14099" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14100" max="14100" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14101" max="14101" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="14102" max="14102" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="14103" max="14103" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14103" max="14103" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14104" max="14104" width="18" style="13" customWidth="1"/>
-    <col min="14105" max="14105" width="7.5" style="13" customWidth="1"/>
-    <col min="14106" max="14106" width="10.5" style="13" customWidth="1"/>
-    <col min="14107" max="14336" width="8.83203125" style="13"/>
-    <col min="14337" max="14337" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14105" width="7.453125" style="13" customWidth="1"/>
+    <col min="14106" max="14106" width="10.453125" style="13" customWidth="1"/>
+    <col min="14107" max="14336" width="8.81640625" style="13"/>
+    <col min="14337" max="14337" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14339" max="14339" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="14340" max="14340" width="7.6640625" style="13" customWidth="1"/>
+    <col min="14340" max="14340" width="7.6328125" style="13" customWidth="1"/>
     <col min="14341" max="14341" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="14342" max="14342" width="8" style="13" customWidth="1"/>
     <col min="14343" max="14343" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="10.33203125" style="13" customWidth="1"/>
-    <col min="14345" max="14345" width="9.5" style="13" customWidth="1"/>
-    <col min="14346" max="14346" width="10.1640625" style="13" customWidth="1"/>
-    <col min="14347" max="14347" width="12.5" style="13" customWidth="1"/>
-    <col min="14348" max="14348" width="6.6640625" style="13" customWidth="1"/>
-    <col min="14349" max="14349" width="6.5" style="13" customWidth="1"/>
-    <col min="14350" max="14350" width="6.33203125" style="13" customWidth="1"/>
-    <col min="14351" max="14351" width="12.5" style="13" customWidth="1"/>
-    <col min="14352" max="14352" width="8.1640625" style="13" customWidth="1"/>
-    <col min="14353" max="14354" width="8.5" style="13" customWidth="1"/>
-    <col min="14355" max="14355" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14356" max="14356" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14357" max="14357" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="10.36328125" style="13" customWidth="1"/>
+    <col min="14345" max="14345" width="9.453125" style="13" customWidth="1"/>
+    <col min="14346" max="14346" width="10.1796875" style="13" customWidth="1"/>
+    <col min="14347" max="14347" width="12.453125" style="13" customWidth="1"/>
+    <col min="14348" max="14348" width="6.6328125" style="13" customWidth="1"/>
+    <col min="14349" max="14349" width="6.453125" style="13" customWidth="1"/>
+    <col min="14350" max="14350" width="6.36328125" style="13" customWidth="1"/>
+    <col min="14351" max="14351" width="12.453125" style="13" customWidth="1"/>
+    <col min="14352" max="14352" width="8.1796875" style="13" customWidth="1"/>
+    <col min="14353" max="14354" width="8.453125" style="13" customWidth="1"/>
+    <col min="14355" max="14355" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14356" max="14356" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14357" max="14357" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="14358" max="14358" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="14359" max="14359" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14359" max="14359" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14360" max="14360" width="18" style="13" customWidth="1"/>
-    <col min="14361" max="14361" width="7.5" style="13" customWidth="1"/>
-    <col min="14362" max="14362" width="10.5" style="13" customWidth="1"/>
-    <col min="14363" max="14592" width="8.83203125" style="13"/>
-    <col min="14593" max="14593" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14361" width="7.453125" style="13" customWidth="1"/>
+    <col min="14362" max="14362" width="10.453125" style="13" customWidth="1"/>
+    <col min="14363" max="14592" width="8.81640625" style="13"/>
+    <col min="14593" max="14593" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14595" max="14595" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="14596" max="14596" width="7.6640625" style="13" customWidth="1"/>
+    <col min="14596" max="14596" width="7.6328125" style="13" customWidth="1"/>
     <col min="14597" max="14597" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="14598" max="14598" width="8" style="13" customWidth="1"/>
     <col min="14599" max="14599" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="10.33203125" style="13" customWidth="1"/>
-    <col min="14601" max="14601" width="9.5" style="13" customWidth="1"/>
-    <col min="14602" max="14602" width="10.1640625" style="13" customWidth="1"/>
-    <col min="14603" max="14603" width="12.5" style="13" customWidth="1"/>
-    <col min="14604" max="14604" width="6.6640625" style="13" customWidth="1"/>
-    <col min="14605" max="14605" width="6.5" style="13" customWidth="1"/>
-    <col min="14606" max="14606" width="6.33203125" style="13" customWidth="1"/>
-    <col min="14607" max="14607" width="12.5" style="13" customWidth="1"/>
-    <col min="14608" max="14608" width="8.1640625" style="13" customWidth="1"/>
-    <col min="14609" max="14610" width="8.5" style="13" customWidth="1"/>
-    <col min="14611" max="14611" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14612" max="14612" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14613" max="14613" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="10.36328125" style="13" customWidth="1"/>
+    <col min="14601" max="14601" width="9.453125" style="13" customWidth="1"/>
+    <col min="14602" max="14602" width="10.1796875" style="13" customWidth="1"/>
+    <col min="14603" max="14603" width="12.453125" style="13" customWidth="1"/>
+    <col min="14604" max="14604" width="6.6328125" style="13" customWidth="1"/>
+    <col min="14605" max="14605" width="6.453125" style="13" customWidth="1"/>
+    <col min="14606" max="14606" width="6.36328125" style="13" customWidth="1"/>
+    <col min="14607" max="14607" width="12.453125" style="13" customWidth="1"/>
+    <col min="14608" max="14608" width="8.1796875" style="13" customWidth="1"/>
+    <col min="14609" max="14610" width="8.453125" style="13" customWidth="1"/>
+    <col min="14611" max="14611" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14612" max="14612" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14613" max="14613" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="14614" max="14614" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="14615" max="14615" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14615" max="14615" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14616" max="14616" width="18" style="13" customWidth="1"/>
-    <col min="14617" max="14617" width="7.5" style="13" customWidth="1"/>
-    <col min="14618" max="14618" width="10.5" style="13" customWidth="1"/>
-    <col min="14619" max="14848" width="8.83203125" style="13"/>
-    <col min="14849" max="14849" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14617" width="7.453125" style="13" customWidth="1"/>
+    <col min="14618" max="14618" width="10.453125" style="13" customWidth="1"/>
+    <col min="14619" max="14848" width="8.81640625" style="13"/>
+    <col min="14849" max="14849" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14851" max="14851" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="14852" max="14852" width="7.6640625" style="13" customWidth="1"/>
+    <col min="14852" max="14852" width="7.6328125" style="13" customWidth="1"/>
     <col min="14853" max="14853" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="14854" max="14854" width="8" style="13" customWidth="1"/>
     <col min="14855" max="14855" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="10.33203125" style="13" customWidth="1"/>
-    <col min="14857" max="14857" width="9.5" style="13" customWidth="1"/>
-    <col min="14858" max="14858" width="10.1640625" style="13" customWidth="1"/>
-    <col min="14859" max="14859" width="12.5" style="13" customWidth="1"/>
-    <col min="14860" max="14860" width="6.6640625" style="13" customWidth="1"/>
-    <col min="14861" max="14861" width="6.5" style="13" customWidth="1"/>
-    <col min="14862" max="14862" width="6.33203125" style="13" customWidth="1"/>
-    <col min="14863" max="14863" width="12.5" style="13" customWidth="1"/>
-    <col min="14864" max="14864" width="8.1640625" style="13" customWidth="1"/>
-    <col min="14865" max="14866" width="8.5" style="13" customWidth="1"/>
-    <col min="14867" max="14867" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14868" max="14868" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14869" max="14869" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="10.36328125" style="13" customWidth="1"/>
+    <col min="14857" max="14857" width="9.453125" style="13" customWidth="1"/>
+    <col min="14858" max="14858" width="10.1796875" style="13" customWidth="1"/>
+    <col min="14859" max="14859" width="12.453125" style="13" customWidth="1"/>
+    <col min="14860" max="14860" width="6.6328125" style="13" customWidth="1"/>
+    <col min="14861" max="14861" width="6.453125" style="13" customWidth="1"/>
+    <col min="14862" max="14862" width="6.36328125" style="13" customWidth="1"/>
+    <col min="14863" max="14863" width="12.453125" style="13" customWidth="1"/>
+    <col min="14864" max="14864" width="8.1796875" style="13" customWidth="1"/>
+    <col min="14865" max="14866" width="8.453125" style="13" customWidth="1"/>
+    <col min="14867" max="14867" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14868" max="14868" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="14869" max="14869" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="14870" max="14870" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="14871" max="14871" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14871" max="14871" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="14872" max="14872" width="18" style="13" customWidth="1"/>
-    <col min="14873" max="14873" width="7.5" style="13" customWidth="1"/>
-    <col min="14874" max="14874" width="10.5" style="13" customWidth="1"/>
-    <col min="14875" max="15104" width="8.83203125" style="13"/>
-    <col min="15105" max="15105" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="14873" max="14873" width="7.453125" style="13" customWidth="1"/>
+    <col min="14874" max="14874" width="10.453125" style="13" customWidth="1"/>
+    <col min="14875" max="15104" width="8.81640625" style="13"/>
+    <col min="15105" max="15105" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15107" max="15107" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="15108" max="15108" width="7.6640625" style="13" customWidth="1"/>
+    <col min="15108" max="15108" width="7.6328125" style="13" customWidth="1"/>
     <col min="15109" max="15109" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="15110" max="15110" width="8" style="13" customWidth="1"/>
     <col min="15111" max="15111" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="10.33203125" style="13" customWidth="1"/>
-    <col min="15113" max="15113" width="9.5" style="13" customWidth="1"/>
-    <col min="15114" max="15114" width="10.1640625" style="13" customWidth="1"/>
-    <col min="15115" max="15115" width="12.5" style="13" customWidth="1"/>
-    <col min="15116" max="15116" width="6.6640625" style="13" customWidth="1"/>
-    <col min="15117" max="15117" width="6.5" style="13" customWidth="1"/>
-    <col min="15118" max="15118" width="6.33203125" style="13" customWidth="1"/>
-    <col min="15119" max="15119" width="12.5" style="13" customWidth="1"/>
-    <col min="15120" max="15120" width="8.1640625" style="13" customWidth="1"/>
-    <col min="15121" max="15122" width="8.5" style="13" customWidth="1"/>
-    <col min="15123" max="15123" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15124" max="15124" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15125" max="15125" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="10.36328125" style="13" customWidth="1"/>
+    <col min="15113" max="15113" width="9.453125" style="13" customWidth="1"/>
+    <col min="15114" max="15114" width="10.1796875" style="13" customWidth="1"/>
+    <col min="15115" max="15115" width="12.453125" style="13" customWidth="1"/>
+    <col min="15116" max="15116" width="6.6328125" style="13" customWidth="1"/>
+    <col min="15117" max="15117" width="6.453125" style="13" customWidth="1"/>
+    <col min="15118" max="15118" width="6.36328125" style="13" customWidth="1"/>
+    <col min="15119" max="15119" width="12.453125" style="13" customWidth="1"/>
+    <col min="15120" max="15120" width="8.1796875" style="13" customWidth="1"/>
+    <col min="15121" max="15122" width="8.453125" style="13" customWidth="1"/>
+    <col min="15123" max="15123" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15124" max="15124" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15125" max="15125" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="15126" max="15126" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="15127" max="15127" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15127" max="15127" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15128" max="15128" width="18" style="13" customWidth="1"/>
-    <col min="15129" max="15129" width="7.5" style="13" customWidth="1"/>
-    <col min="15130" max="15130" width="10.5" style="13" customWidth="1"/>
-    <col min="15131" max="15360" width="8.83203125" style="13"/>
-    <col min="15361" max="15361" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15129" width="7.453125" style="13" customWidth="1"/>
+    <col min="15130" max="15130" width="10.453125" style="13" customWidth="1"/>
+    <col min="15131" max="15360" width="8.81640625" style="13"/>
+    <col min="15361" max="15361" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15363" max="15363" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="15364" max="15364" width="7.6640625" style="13" customWidth="1"/>
+    <col min="15364" max="15364" width="7.6328125" style="13" customWidth="1"/>
     <col min="15365" max="15365" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="15366" max="15366" width="8" style="13" customWidth="1"/>
     <col min="15367" max="15367" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="10.33203125" style="13" customWidth="1"/>
-    <col min="15369" max="15369" width="9.5" style="13" customWidth="1"/>
-    <col min="15370" max="15370" width="10.1640625" style="13" customWidth="1"/>
-    <col min="15371" max="15371" width="12.5" style="13" customWidth="1"/>
-    <col min="15372" max="15372" width="6.6640625" style="13" customWidth="1"/>
-    <col min="15373" max="15373" width="6.5" style="13" customWidth="1"/>
-    <col min="15374" max="15374" width="6.33203125" style="13" customWidth="1"/>
-    <col min="15375" max="15375" width="12.5" style="13" customWidth="1"/>
-    <col min="15376" max="15376" width="8.1640625" style="13" customWidth="1"/>
-    <col min="15377" max="15378" width="8.5" style="13" customWidth="1"/>
-    <col min="15379" max="15379" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15380" max="15380" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15381" max="15381" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="10.36328125" style="13" customWidth="1"/>
+    <col min="15369" max="15369" width="9.453125" style="13" customWidth="1"/>
+    <col min="15370" max="15370" width="10.1796875" style="13" customWidth="1"/>
+    <col min="15371" max="15371" width="12.453125" style="13" customWidth="1"/>
+    <col min="15372" max="15372" width="6.6328125" style="13" customWidth="1"/>
+    <col min="15373" max="15373" width="6.453125" style="13" customWidth="1"/>
+    <col min="15374" max="15374" width="6.36328125" style="13" customWidth="1"/>
+    <col min="15375" max="15375" width="12.453125" style="13" customWidth="1"/>
+    <col min="15376" max="15376" width="8.1796875" style="13" customWidth="1"/>
+    <col min="15377" max="15378" width="8.453125" style="13" customWidth="1"/>
+    <col min="15379" max="15379" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15380" max="15380" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15381" max="15381" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="15382" max="15382" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="15383" max="15383" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15383" max="15383" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15384" max="15384" width="18" style="13" customWidth="1"/>
-    <col min="15385" max="15385" width="7.5" style="13" customWidth="1"/>
-    <col min="15386" max="15386" width="10.5" style="13" customWidth="1"/>
-    <col min="15387" max="15616" width="8.83203125" style="13"/>
-    <col min="15617" max="15617" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15385" width="7.453125" style="13" customWidth="1"/>
+    <col min="15386" max="15386" width="10.453125" style="13" customWidth="1"/>
+    <col min="15387" max="15616" width="8.81640625" style="13"/>
+    <col min="15617" max="15617" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15619" max="15619" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="15620" max="15620" width="7.6640625" style="13" customWidth="1"/>
+    <col min="15620" max="15620" width="7.6328125" style="13" customWidth="1"/>
     <col min="15621" max="15621" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="15622" max="15622" width="8" style="13" customWidth="1"/>
     <col min="15623" max="15623" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="10.33203125" style="13" customWidth="1"/>
-    <col min="15625" max="15625" width="9.5" style="13" customWidth="1"/>
-    <col min="15626" max="15626" width="10.1640625" style="13" customWidth="1"/>
-    <col min="15627" max="15627" width="12.5" style="13" customWidth="1"/>
-    <col min="15628" max="15628" width="6.6640625" style="13" customWidth="1"/>
-    <col min="15629" max="15629" width="6.5" style="13" customWidth="1"/>
-    <col min="15630" max="15630" width="6.33203125" style="13" customWidth="1"/>
-    <col min="15631" max="15631" width="12.5" style="13" customWidth="1"/>
-    <col min="15632" max="15632" width="8.1640625" style="13" customWidth="1"/>
-    <col min="15633" max="15634" width="8.5" style="13" customWidth="1"/>
-    <col min="15635" max="15635" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15636" max="15636" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15637" max="15637" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="10.36328125" style="13" customWidth="1"/>
+    <col min="15625" max="15625" width="9.453125" style="13" customWidth="1"/>
+    <col min="15626" max="15626" width="10.1796875" style="13" customWidth="1"/>
+    <col min="15627" max="15627" width="12.453125" style="13" customWidth="1"/>
+    <col min="15628" max="15628" width="6.6328125" style="13" customWidth="1"/>
+    <col min="15629" max="15629" width="6.453125" style="13" customWidth="1"/>
+    <col min="15630" max="15630" width="6.36328125" style="13" customWidth="1"/>
+    <col min="15631" max="15631" width="12.453125" style="13" customWidth="1"/>
+    <col min="15632" max="15632" width="8.1796875" style="13" customWidth="1"/>
+    <col min="15633" max="15634" width="8.453125" style="13" customWidth="1"/>
+    <col min="15635" max="15635" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15636" max="15636" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15637" max="15637" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="15638" max="15638" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="15639" max="15639" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15639" max="15639" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15640" max="15640" width="18" style="13" customWidth="1"/>
-    <col min="15641" max="15641" width="7.5" style="13" customWidth="1"/>
-    <col min="15642" max="15642" width="10.5" style="13" customWidth="1"/>
-    <col min="15643" max="15872" width="8.83203125" style="13"/>
-    <col min="15873" max="15873" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15641" width="7.453125" style="13" customWidth="1"/>
+    <col min="15642" max="15642" width="10.453125" style="13" customWidth="1"/>
+    <col min="15643" max="15872" width="8.81640625" style="13"/>
+    <col min="15873" max="15873" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15875" max="15875" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="15876" max="15876" width="7.6640625" style="13" customWidth="1"/>
+    <col min="15876" max="15876" width="7.6328125" style="13" customWidth="1"/>
     <col min="15877" max="15877" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="15878" max="15878" width="8" style="13" customWidth="1"/>
     <col min="15879" max="15879" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="10.33203125" style="13" customWidth="1"/>
-    <col min="15881" max="15881" width="9.5" style="13" customWidth="1"/>
-    <col min="15882" max="15882" width="10.1640625" style="13" customWidth="1"/>
-    <col min="15883" max="15883" width="12.5" style="13" customWidth="1"/>
-    <col min="15884" max="15884" width="6.6640625" style="13" customWidth="1"/>
-    <col min="15885" max="15885" width="6.5" style="13" customWidth="1"/>
-    <col min="15886" max="15886" width="6.33203125" style="13" customWidth="1"/>
-    <col min="15887" max="15887" width="12.5" style="13" customWidth="1"/>
-    <col min="15888" max="15888" width="8.1640625" style="13" customWidth="1"/>
-    <col min="15889" max="15890" width="8.5" style="13" customWidth="1"/>
-    <col min="15891" max="15891" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15892" max="15892" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15893" max="15893" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="10.36328125" style="13" customWidth="1"/>
+    <col min="15881" max="15881" width="9.453125" style="13" customWidth="1"/>
+    <col min="15882" max="15882" width="10.1796875" style="13" customWidth="1"/>
+    <col min="15883" max="15883" width="12.453125" style="13" customWidth="1"/>
+    <col min="15884" max="15884" width="6.6328125" style="13" customWidth="1"/>
+    <col min="15885" max="15885" width="6.453125" style="13" customWidth="1"/>
+    <col min="15886" max="15886" width="6.36328125" style="13" customWidth="1"/>
+    <col min="15887" max="15887" width="12.453125" style="13" customWidth="1"/>
+    <col min="15888" max="15888" width="8.1796875" style="13" customWidth="1"/>
+    <col min="15889" max="15890" width="8.453125" style="13" customWidth="1"/>
+    <col min="15891" max="15891" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15892" max="15892" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15893" max="15893" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="15894" max="15894" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="15895" max="15895" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15895" max="15895" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="15896" max="15896" width="18" style="13" customWidth="1"/>
-    <col min="15897" max="15897" width="7.5" style="13" customWidth="1"/>
-    <col min="15898" max="15898" width="10.5" style="13" customWidth="1"/>
-    <col min="15899" max="16128" width="8.83203125" style="13"/>
-    <col min="16129" max="16129" width="6.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="4.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15897" max="15897" width="7.453125" style="13" customWidth="1"/>
+    <col min="15898" max="15898" width="10.453125" style="13" customWidth="1"/>
+    <col min="15899" max="16128" width="8.81640625" style="13"/>
+    <col min="16129" max="16129" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="4.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="16131" max="16131" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="16132" max="16132" width="7.6640625" style="13" customWidth="1"/>
+    <col min="16132" max="16132" width="7.6328125" style="13" customWidth="1"/>
     <col min="16133" max="16133" width="6" style="13" bestFit="1" customWidth="1"/>
     <col min="16134" max="16134" width="8" style="13" customWidth="1"/>
     <col min="16135" max="16135" width="8" style="13" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="10.33203125" style="13" customWidth="1"/>
-    <col min="16137" max="16137" width="9.5" style="13" customWidth="1"/>
-    <col min="16138" max="16138" width="10.1640625" style="13" customWidth="1"/>
-    <col min="16139" max="16139" width="12.5" style="13" customWidth="1"/>
-    <col min="16140" max="16140" width="6.6640625" style="13" customWidth="1"/>
-    <col min="16141" max="16141" width="6.5" style="13" customWidth="1"/>
-    <col min="16142" max="16142" width="6.33203125" style="13" customWidth="1"/>
-    <col min="16143" max="16143" width="12.5" style="13" customWidth="1"/>
-    <col min="16144" max="16144" width="8.1640625" style="13" customWidth="1"/>
-    <col min="16145" max="16146" width="8.5" style="13" customWidth="1"/>
-    <col min="16147" max="16147" width="9.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16148" max="16148" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16149" max="16149" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="10.36328125" style="13" customWidth="1"/>
+    <col min="16137" max="16137" width="9.453125" style="13" customWidth="1"/>
+    <col min="16138" max="16138" width="10.1796875" style="13" customWidth="1"/>
+    <col min="16139" max="16139" width="12.453125" style="13" customWidth="1"/>
+    <col min="16140" max="16140" width="6.6328125" style="13" customWidth="1"/>
+    <col min="16141" max="16141" width="6.453125" style="13" customWidth="1"/>
+    <col min="16142" max="16142" width="6.36328125" style="13" customWidth="1"/>
+    <col min="16143" max="16143" width="12.453125" style="13" customWidth="1"/>
+    <col min="16144" max="16144" width="8.1796875" style="13" customWidth="1"/>
+    <col min="16145" max="16146" width="8.453125" style="13" customWidth="1"/>
+    <col min="16147" max="16147" width="9.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="16148" max="16148" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="16149" max="16149" width="10.36328125" style="13" bestFit="1" customWidth="1"/>
     <col min="16150" max="16150" width="10" style="13" bestFit="1" customWidth="1"/>
-    <col min="16151" max="16151" width="7.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="16151" max="16151" width="7.453125" style="13" bestFit="1" customWidth="1"/>
     <col min="16152" max="16152" width="18" style="13" customWidth="1"/>
-    <col min="16153" max="16153" width="7.5" style="13" customWidth="1"/>
-    <col min="16154" max="16154" width="10.5" style="13" customWidth="1"/>
-    <col min="16155" max="16384" width="8.83203125" style="13"/>
+    <col min="16153" max="16153" width="7.453125" style="13" customWidth="1"/>
+    <col min="16154" max="16154" width="10.453125" style="13" customWidth="1"/>
+    <col min="16155" max="16384" width="8.81640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:30" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -3906,7 +3906,7 @@
       <c r="AC2" s="12"/>
       <c r="AD2" s="12"/>
     </row>
-    <row r="3" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="AC3" s="12"/>
       <c r="AD3" s="12"/>
     </row>
-    <row r="4" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
@@ -4074,7 +4074,7 @@
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
     </row>
-    <row r="5" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -4158,7 +4158,7 @@
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
     </row>
-    <row r="6" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
@@ -4242,7 +4242,7 @@
       <c r="AC6" s="12"/>
       <c r="AD6" s="12"/>
     </row>
-    <row r="7" spans="1:30" ht="33" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" ht="40" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
@@ -4326,7 +4326,7 @@
       <c r="AC7" s="12"/>
       <c r="AD7" s="12"/>
     </row>
-    <row r="8" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -4410,7 +4410,7 @@
       <c r="AC8" s="12"/>
       <c r="AD8" s="12"/>
     </row>
-    <row r="9" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
@@ -4494,7 +4494,7 @@
       <c r="AC9" s="12"/>
       <c r="AD9" s="12"/>
     </row>
-    <row r="10" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
@@ -4578,7 +4578,7 @@
       <c r="AC10" s="12"/>
       <c r="AD10" s="12"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
@@ -4662,7 +4662,7 @@
       <c r="AC11" s="12"/>
       <c r="AD11" s="12"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
@@ -4746,7 +4746,7 @@
       <c r="AC12" s="12"/>
       <c r="AD12" s="12"/>
     </row>
-    <row r="13" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -4830,7 +4830,7 @@
       <c r="AC13" s="12"/>
       <c r="AD13" s="12"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
@@ -4914,7 +4914,7 @@
       <c r="AC14" s="12"/>
       <c r="AD14" s="12"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -4998,7 +4998,7 @@
       <c r="AC15" s="12"/>
       <c r="AD15" s="12"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -5082,7 +5082,7 @@
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
     </row>
-    <row r="17" spans="1:30" ht="33" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
@@ -5166,7 +5166,7 @@
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
     </row>
-    <row r="18" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
@@ -5250,7 +5250,7 @@
       <c r="AC18" s="12"/>
       <c r="AD18" s="12"/>
     </row>
-    <row r="19" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="AC19" s="12"/>
       <c r="AD19" s="12"/>
     </row>
-    <row r="20" spans="1:30" ht="33" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:30" ht="40" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -5418,7 +5418,7 @@
       <c r="AC20" s="12"/>
       <c r="AD20" s="12"/>
     </row>
-    <row r="21" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
@@ -5502,7 +5502,7 @@
       <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
     </row>
-    <row r="22" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
@@ -5586,7 +5586,7 @@
       <c r="AC22" s="12"/>
       <c r="AD22" s="12"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>26</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
@@ -5750,7 +5750,7 @@
       <c r="AC24" s="12"/>
       <c r="AD24" s="12"/>
     </row>
-    <row r="25" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>26</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -5914,7 +5914,7 @@
       <c r="AC26" s="12"/>
       <c r="AD26" s="12"/>
     </row>
-    <row r="27" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -5998,7 +5998,7 @@
       <c r="AC27" s="12"/>
       <c r="AD27" s="12"/>
     </row>
-    <row r="28" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="AC28" s="12"/>
       <c r="AD28" s="12"/>
     </row>
-    <row r="29" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>26</v>
       </c>
@@ -6166,7 +6166,7 @@
       <c r="AC29" s="12"/>
       <c r="AD29" s="12"/>
     </row>
-    <row r="30" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>26</v>
       </c>
@@ -6250,7 +6250,7 @@
       <c r="AC30" s="12"/>
       <c r="AD30" s="12"/>
     </row>
-    <row r="31" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>26</v>
       </c>
@@ -6334,7 +6334,7 @@
       <c r="AC31" s="12"/>
       <c r="AD31" s="12"/>
     </row>
-    <row r="32" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -6418,7 +6418,7 @@
       <c r="AC32" s="17"/>
       <c r="AD32" s="17"/>
     </row>
-    <row r="33" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>26</v>
       </c>
@@ -6502,7 +6502,7 @@
       <c r="AC33" s="17"/>
       <c r="AD33" s="17"/>
     </row>
-    <row r="34" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>26</v>
       </c>
@@ -6586,7 +6586,7 @@
       <c r="AC34" s="17"/>
       <c r="AD34" s="17"/>
     </row>
-    <row r="35" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>26</v>
       </c>
@@ -6670,7 +6670,7 @@
       <c r="AC35" s="17"/>
       <c r="AD35" s="17"/>
     </row>
-    <row r="36" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>26</v>
       </c>
@@ -6754,7 +6754,7 @@
       <c r="AC36" s="17"/>
       <c r="AD36" s="17"/>
     </row>
-    <row r="37" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>26</v>
       </c>
@@ -6838,7 +6838,7 @@
       <c r="AC37" s="17"/>
       <c r="AD37" s="17"/>
     </row>
-    <row r="38" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>26</v>
       </c>
@@ -6922,7 +6922,7 @@
       <c r="AC38" s="17"/>
       <c r="AD38" s="17"/>
     </row>
-    <row r="39" spans="1:30" ht="33" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>26</v>
       </c>
@@ -7006,7 +7006,7 @@
       <c r="AC39" s="17"/>
       <c r="AD39" s="17"/>
     </row>
-    <row r="40" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>26</v>
       </c>
@@ -7090,7 +7090,7 @@
       <c r="AC40" s="17"/>
       <c r="AD40" s="17"/>
     </row>
-    <row r="41" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>26</v>
       </c>
@@ -7174,7 +7174,7 @@
       <c r="AC41" s="17"/>
       <c r="AD41" s="17"/>
     </row>
-    <row r="42" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>26</v>
       </c>
@@ -7258,7 +7258,7 @@
       <c r="AC42" s="17"/>
       <c r="AD42" s="17"/>
     </row>
-    <row r="43" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>26</v>
       </c>
@@ -7342,7 +7342,7 @@
       <c r="AC43" s="17"/>
       <c r="AD43" s="17"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>26</v>
       </c>
@@ -7426,7 +7426,7 @@
       <c r="AC44" s="17"/>
       <c r="AD44" s="17"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>26</v>
       </c>
@@ -7510,7 +7510,7 @@
       <c r="AC45" s="17"/>
       <c r="AD45" s="17"/>
     </row>
-    <row r="46" spans="1:30" ht="33" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>26</v>
       </c>
@@ -7594,7 +7594,7 @@
       <c r="AC46" s="17"/>
       <c r="AD46" s="17"/>
     </row>
-    <row r="47" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>26</v>
       </c>
@@ -7678,7 +7678,7 @@
       <c r="AC47" s="17"/>
       <c r="AD47" s="17"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>26</v>
       </c>
@@ -7762,7 +7762,7 @@
       <c r="AC48" s="17"/>
       <c r="AD48" s="17"/>
     </row>
-    <row r="49" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>26</v>
       </c>
@@ -7846,7 +7846,7 @@
       <c r="AC49" s="17"/>
       <c r="AD49" s="17"/>
     </row>
-    <row r="50" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>26</v>
       </c>
@@ -7930,7 +7930,7 @@
       <c r="AC50" s="17"/>
       <c r="AD50" s="17"/>
     </row>
-    <row r="51" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>26</v>
       </c>
@@ -8014,7 +8014,7 @@
       <c r="AC51" s="17"/>
       <c r="AD51" s="17"/>
     </row>
-    <row r="52" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>26</v>
       </c>
@@ -8098,7 +8098,7 @@
       <c r="AC52" s="17"/>
       <c r="AD52" s="17"/>
     </row>
-    <row r="53" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>26</v>
       </c>
@@ -8182,7 +8182,7 @@
       <c r="AC53" s="17"/>
       <c r="AD53" s="17"/>
     </row>
-    <row r="54" spans="1:30" ht="33" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>26</v>
       </c>
@@ -8266,7 +8266,7 @@
       <c r="AC54" s="17"/>
       <c r="AD54" s="17"/>
     </row>
-    <row r="55" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>26</v>
       </c>
@@ -8350,7 +8350,7 @@
       <c r="AC55" s="17"/>
       <c r="AD55" s="17"/>
     </row>
-    <row r="56" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>26</v>
       </c>
@@ -8363,8 +8363,8 @@
       <c r="D56" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>120</v>
+      <c r="E56" s="38" t="s">
+        <v>489</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>28</v>
@@ -8434,7 +8434,7 @@
       <c r="AC56" s="17"/>
       <c r="AD56" s="17"/>
     </row>
-    <row r="57" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>26</v>
       </c>
@@ -8518,7 +8518,7 @@
       <c r="AC57" s="17"/>
       <c r="AD57" s="17"/>
     </row>
-    <row r="58" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>26</v>
       </c>
@@ -8602,7 +8602,7 @@
       <c r="AC58" s="17"/>
       <c r="AD58" s="17"/>
     </row>
-    <row r="59" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>26</v>
       </c>
@@ -8686,7 +8686,7 @@
       <c r="AC59" s="17"/>
       <c r="AD59" s="17"/>
     </row>
-    <row r="60" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>26</v>
       </c>
@@ -8770,7 +8770,7 @@
       <c r="AC60" s="17"/>
       <c r="AD60" s="17"/>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>26</v>
       </c>
@@ -8854,7 +8854,7 @@
       <c r="AC61" s="17"/>
       <c r="AD61" s="17"/>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A62" s="21" t="s">
         <v>26</v>
       </c>
@@ -8938,7 +8938,7 @@
       <c r="AC62" s="12"/>
       <c r="AD62" s="12"/>
     </row>
-    <row r="63" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A63" s="21" t="s">
         <v>26</v>
       </c>
@@ -9022,7 +9022,7 @@
       <c r="AC63" s="12"/>
       <c r="AD63" s="12"/>
     </row>
-    <row r="64" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A64" s="21" t="s">
         <v>26</v>
       </c>
@@ -9106,7 +9106,7 @@
       <c r="AC64" s="12"/>
       <c r="AD64" s="12"/>
     </row>
-    <row r="65" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A65" s="21" t="s">
         <v>26</v>
       </c>
@@ -9190,7 +9190,7 @@
       <c r="AC65" s="12"/>
       <c r="AD65" s="12"/>
     </row>
-    <row r="66" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
         <v>26</v>
       </c>
@@ -9274,7 +9274,7 @@
       <c r="AC66" s="12"/>
       <c r="AD66" s="12"/>
     </row>
-    <row r="67" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A67" s="21" t="s">
         <v>26</v>
       </c>
@@ -9358,7 +9358,7 @@
       <c r="AC67" s="12"/>
       <c r="AD67" s="12"/>
     </row>
-    <row r="68" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A68" s="21" t="s">
         <v>26</v>
       </c>
@@ -9442,7 +9442,7 @@
       <c r="AC68" s="12"/>
       <c r="AD68" s="12"/>
     </row>
-    <row r="69" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:30" ht="30" x14ac:dyDescent="0.2">
       <c r="A69" s="21" t="s">
         <v>26</v>
       </c>
@@ -9526,7 +9526,7 @@
       <c r="AC69" s="12"/>
       <c r="AD69" s="12"/>
     </row>
-    <row r="70" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A70" s="21" t="s">
         <v>26</v>
       </c>
@@ -9610,7 +9610,7 @@
       <c r="AC70" s="12"/>
       <c r="AD70" s="12"/>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A71" s="21" t="s">
         <v>26</v>
       </c>
@@ -9694,7 +9694,7 @@
       <c r="AC71" s="12"/>
       <c r="AD71" s="12"/>
     </row>
-    <row r="72" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A72" s="21" t="s">
         <v>26</v>
       </c>
@@ -9778,7 +9778,7 @@
       <c r="AC72" s="12"/>
       <c r="AD72" s="12"/>
     </row>
-    <row r="73" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A73" s="21" t="s">
         <v>26</v>
       </c>
@@ -9862,7 +9862,7 @@
       <c r="AC73" s="12"/>
       <c r="AD73" s="12"/>
     </row>
-    <row r="74" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A74" s="21" t="s">
         <v>26</v>
       </c>
@@ -9946,7 +9946,7 @@
       <c r="AC74" s="12"/>
       <c r="AD74" s="12"/>
     </row>
-    <row r="75" spans="1:30" ht="22" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:30" ht="20" x14ac:dyDescent="0.2">
       <c r="A75" s="21" t="s">
         <v>26</v>
       </c>
@@ -10030,44 +10030,43 @@
       <c r="AC75" s="12"/>
       <c r="AD75" s="12"/>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
       <c r="Q76" s="37"/>
       <c r="T76" s="45"/>
       <c r="U76" s="6"/>
       <c r="V76" s="37"/>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
       <c r="Q77" s="37"/>
       <c r="T77" s="45"/>
       <c r="V77" s="37"/>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="Q78" s="37"/>
       <c r="T78" s="45"/>
       <c r="V78" s="37"/>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="Q79" s="37"/>
       <c r="T79" s="45"/>
       <c r="V79" s="37"/>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="Q80" s="37"/>
       <c r="T80" s="45"/>
       <c r="V80" s="37"/>
     </row>
-    <row r="81" spans="17:22" x14ac:dyDescent="0.15">
+    <row r="81" spans="17:22" x14ac:dyDescent="0.2">
       <c r="Q81" s="37"/>
       <c r="T81" s="45"/>
       <c r="V81" s="37"/>
     </row>
-    <row r="82" spans="17:22" x14ac:dyDescent="0.15">
+    <row r="82" spans="17:22" x14ac:dyDescent="0.2">
       <c r="Q82" s="37"/>
       <c r="T82" s="45"/>
       <c r="V82" s="37"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:WWH82"/>
   <sortState ref="A2:WWH82">
     <sortCondition ref="D2:D82"/>
     <sortCondition ref="E2:E82"/>

</xml_diff>